<commit_message>
Correzioni manuali VDA, correzioni a LOM e TAA
</commit_message>
<xml_diff>
--- a/external/correzioni/TAA2_edit.xlsx
+++ b/external/correzioni/TAA2_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenicoli/Local_Workspace/TesiMag/external/correzioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C4E96F-1483-894B-B3B7-D8309059F670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACD903F-B72F-E644-975A-7859B2A63D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" xr2:uid="{3DA680EC-228F-A245-943E-654A6BC08959}"/>
   </bookViews>
@@ -3660,7 +3660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3683,15 +3683,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4116,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813C1DE2-AC54-2F42-A800-EF25757F6AF3}">
   <dimension ref="A1:AH412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E390" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E269" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="AB405" sqref="AB405"/>
     </sheetView>
@@ -4150,7 +4144,7 @@
     <col min="27" max="27" width="16.5" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="13.83203125" customWidth="1"/>
     <col min="32" max="32" width="14.83203125" customWidth="1"/>
-    <col min="33" max="33" width="0" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="9.83203125" customWidth="1"/>
     <col min="34" max="34" width="69.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10571,13 +10565,7 @@
       <c r="AA73" t="s">
         <v>36</v>
       </c>
-      <c r="AB73" s="12"/>
-      <c r="AC73" s="12"/>
-      <c r="AD73" s="12"/>
-      <c r="AE73" s="12"/>
-      <c r="AF73" s="12"/>
-      <c r="AG73" s="12"/>
-      <c r="AH73" s="13"/>
+      <c r="AH73" s="6"/>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A74">
@@ -10757,13 +10745,7 @@
       <c r="AA75" t="s">
         <v>36</v>
       </c>
-      <c r="AB75" s="12"/>
-      <c r="AC75" s="12"/>
-      <c r="AD75" s="12"/>
-      <c r="AE75" s="12"/>
-      <c r="AF75" s="12"/>
-      <c r="AG75" s="12"/>
-      <c r="AH75" s="13"/>
+      <c r="AH75" s="6"/>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A76">
@@ -10848,13 +10830,7 @@
       <c r="AA76" t="s">
         <v>36</v>
       </c>
-      <c r="AB76" s="12"/>
-      <c r="AC76" s="12"/>
-      <c r="AD76" s="12"/>
-      <c r="AE76" s="12"/>
-      <c r="AF76" s="12"/>
-      <c r="AG76" s="12"/>
-      <c r="AH76" s="13"/>
+      <c r="AH76" s="6"/>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -11034,15 +11010,10 @@
       <c r="AA78" t="s">
         <v>36</v>
       </c>
-      <c r="AB78" s="12"/>
-      <c r="AC78" s="12"/>
-      <c r="AD78" s="12">
+      <c r="AD78">
         <v>1202</v>
       </c>
-      <c r="AE78" s="12"/>
-      <c r="AF78" s="12"/>
-      <c r="AG78" s="12"/>
-      <c r="AH78" s="13"/>
+      <c r="AH78" s="6"/>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -11127,15 +11098,10 @@
       <c r="AA79" t="s">
         <v>36</v>
       </c>
-      <c r="AB79" s="12"/>
-      <c r="AC79" s="12"/>
-      <c r="AD79" s="12">
+      <c r="AD79">
         <v>462</v>
       </c>
-      <c r="AE79" s="12"/>
-      <c r="AF79" s="12"/>
-      <c r="AG79" s="12"/>
-      <c r="AH79" s="13"/>
+      <c r="AH79" s="6"/>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -11220,13 +11186,7 @@
       <c r="AA80" t="s">
         <v>36</v>
       </c>
-      <c r="AB80" s="12"/>
-      <c r="AC80" s="12"/>
-      <c r="AD80" s="12"/>
-      <c r="AE80" s="12"/>
-      <c r="AF80" s="12"/>
-      <c r="AG80" s="12"/>
-      <c r="AH80" s="13"/>
+      <c r="AH80" s="6"/>
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A81">
@@ -11311,13 +11271,7 @@
       <c r="AA81" t="s">
         <v>36</v>
       </c>
-      <c r="AB81" s="12"/>
-      <c r="AC81" s="12"/>
-      <c r="AD81" s="12"/>
-      <c r="AE81" s="12"/>
-      <c r="AF81" s="12"/>
-      <c r="AG81" s="12"/>
-      <c r="AH81" s="13"/>
+      <c r="AH81" s="6"/>
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A82">
@@ -11501,13 +11455,7 @@
       <c r="AA83" t="s">
         <v>36</v>
       </c>
-      <c r="AB83" s="12"/>
-      <c r="AC83" s="12"/>
-      <c r="AD83" s="12"/>
-      <c r="AE83" s="12"/>
-      <c r="AF83" s="12"/>
-      <c r="AG83" s="12"/>
-      <c r="AH83" s="13"/>
+      <c r="AH83" s="6"/>
     </row>
     <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -11592,13 +11540,7 @@
       <c r="AA84" t="s">
         <v>36</v>
       </c>
-      <c r="AB84" s="12"/>
-      <c r="AC84" s="12"/>
-      <c r="AD84" s="12"/>
-      <c r="AE84" s="12"/>
-      <c r="AF84" s="12"/>
-      <c r="AG84" s="12"/>
-      <c r="AH84" s="13"/>
+      <c r="AH84" s="6"/>
     </row>
     <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A85">
@@ -11683,17 +11625,13 @@
       <c r="AA85" t="s">
         <v>36</v>
       </c>
-      <c r="AB85" s="12">
+      <c r="AB85">
         <v>11.31837</v>
       </c>
-      <c r="AC85" s="12">
+      <c r="AC85">
         <v>46.840809999999998</v>
       </c>
-      <c r="AD85" s="12"/>
-      <c r="AE85" s="12"/>
-      <c r="AF85" s="12"/>
-      <c r="AG85" s="12"/>
-      <c r="AH85" s="13"/>
+      <c r="AH85" s="6"/>
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -11778,13 +11716,7 @@
       <c r="AA86" t="s">
         <v>36</v>
       </c>
-      <c r="AB86" s="12"/>
-      <c r="AC86" s="12"/>
-      <c r="AD86" s="12"/>
-      <c r="AE86" s="12"/>
-      <c r="AF86" s="12"/>
-      <c r="AG86" s="12"/>
-      <c r="AH86" s="13"/>
+      <c r="AH86" s="6"/>
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A87">
@@ -11869,13 +11801,7 @@
       <c r="AA87" t="s">
         <v>36</v>
       </c>
-      <c r="AB87" s="12"/>
-      <c r="AC87" s="12"/>
-      <c r="AD87" s="12"/>
-      <c r="AE87" s="12"/>
-      <c r="AF87" s="12"/>
-      <c r="AG87" s="12"/>
-      <c r="AH87" s="13"/>
+      <c r="AH87" s="6"/>
     </row>
     <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A88">
@@ -12055,13 +11981,7 @@
       <c r="AA89" t="s">
         <v>36</v>
       </c>
-      <c r="AB89" s="12"/>
-      <c r="AC89" s="12"/>
-      <c r="AD89" s="12"/>
-      <c r="AE89" s="12"/>
-      <c r="AF89" s="12"/>
-      <c r="AG89" s="12"/>
-      <c r="AH89" s="13"/>
+      <c r="AH89" s="6"/>
     </row>
     <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -12146,13 +12066,7 @@
       <c r="AA90" t="s">
         <v>36</v>
       </c>
-      <c r="AB90" s="12"/>
-      <c r="AC90" s="12"/>
-      <c r="AD90" s="12"/>
-      <c r="AE90" s="12"/>
-      <c r="AF90" s="12"/>
-      <c r="AG90" s="12"/>
-      <c r="AH90" s="13"/>
+      <c r="AH90" s="6"/>
     </row>
     <row r="91" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A91">
@@ -12237,13 +12151,7 @@
       <c r="AA91" t="s">
         <v>36</v>
       </c>
-      <c r="AB91" s="12"/>
-      <c r="AC91" s="12"/>
-      <c r="AD91" s="12"/>
-      <c r="AE91" s="12"/>
-      <c r="AF91" s="12"/>
-      <c r="AG91" s="12"/>
-      <c r="AH91" s="13"/>
+      <c r="AH91" s="6"/>
     </row>
     <row r="92" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A92">
@@ -12328,13 +12236,7 @@
       <c r="AA92" t="s">
         <v>36</v>
       </c>
-      <c r="AB92" s="12"/>
-      <c r="AC92" s="12"/>
-      <c r="AD92" s="12"/>
-      <c r="AE92" s="12"/>
-      <c r="AF92" s="12"/>
-      <c r="AG92" s="12"/>
-      <c r="AH92" s="13"/>
+      <c r="AH92" s="6"/>
     </row>
     <row r="93" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A93">
@@ -12419,13 +12321,7 @@
       <c r="AA93" t="s">
         <v>36</v>
       </c>
-      <c r="AB93" s="12"/>
-      <c r="AC93" s="12"/>
-      <c r="AD93" s="12"/>
-      <c r="AE93" s="12"/>
-      <c r="AF93" s="12"/>
-      <c r="AG93" s="12"/>
-      <c r="AH93" s="13"/>
+      <c r="AH93" s="6"/>
     </row>
     <row r="94" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A94">
@@ -12510,13 +12406,7 @@
       <c r="AA94" t="s">
         <v>36</v>
       </c>
-      <c r="AB94" s="12"/>
-      <c r="AC94" s="12"/>
-      <c r="AD94" s="12"/>
-      <c r="AE94" s="12"/>
-      <c r="AF94" s="12"/>
-      <c r="AG94" s="12"/>
-      <c r="AH94" s="13"/>
+      <c r="AH94" s="6"/>
     </row>
     <row r="95" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A95">
@@ -12601,13 +12491,7 @@
       <c r="AA95" t="s">
         <v>36</v>
       </c>
-      <c r="AB95" s="12"/>
-      <c r="AC95" s="12"/>
-      <c r="AD95" s="12"/>
-      <c r="AE95" s="12"/>
-      <c r="AF95" s="12"/>
-      <c r="AG95" s="12"/>
-      <c r="AH95" s="13"/>
+      <c r="AH95" s="6"/>
     </row>
     <row r="96" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A96">
@@ -12692,19 +12576,16 @@
       <c r="AA96" t="s">
         <v>36</v>
       </c>
-      <c r="AB96" s="12">
+      <c r="AB96">
         <v>10.725752</v>
       </c>
-      <c r="AC96" s="12">
+      <c r="AC96">
         <v>46.509135999999998</v>
       </c>
-      <c r="AD96" s="12">
+      <c r="AD96">
         <v>1856</v>
       </c>
-      <c r="AE96" s="12"/>
-      <c r="AF96" s="12"/>
-      <c r="AG96" s="12"/>
-      <c r="AH96" s="13"/>
+      <c r="AH96" s="6"/>
     </row>
     <row r="97" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A97">
@@ -13157,13 +13038,7 @@
       <c r="AA101" t="s">
         <v>36</v>
       </c>
-      <c r="AB101" s="12"/>
-      <c r="AC101" s="12"/>
-      <c r="AD101" s="12"/>
-      <c r="AE101" s="12"/>
-      <c r="AF101" s="12"/>
-      <c r="AG101" s="12"/>
-      <c r="AH101" s="13"/>
+      <c r="AH101" s="6"/>
     </row>
     <row r="102" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A102">
@@ -13339,13 +13214,7 @@
       <c r="AA103" t="s">
         <v>36</v>
       </c>
-      <c r="AB103" s="12"/>
-      <c r="AC103" s="12"/>
-      <c r="AD103" s="12"/>
-      <c r="AE103" s="12"/>
-      <c r="AF103" s="12"/>
-      <c r="AG103" s="12"/>
-      <c r="AH103" s="13" t="s">
+      <c r="AH103" s="6" t="s">
         <v>1171</v>
       </c>
     </row>
@@ -13432,13 +13301,7 @@
       <c r="AA104" t="s">
         <v>36</v>
       </c>
-      <c r="AB104" s="12"/>
-      <c r="AC104" s="12"/>
-      <c r="AD104" s="12"/>
-      <c r="AE104" s="12"/>
-      <c r="AF104" s="12"/>
-      <c r="AG104" s="12"/>
-      <c r="AH104" s="13"/>
+      <c r="AH104" s="6"/>
     </row>
     <row r="105" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A105">
@@ -13523,13 +13386,7 @@
       <c r="AA105" t="s">
         <v>36</v>
       </c>
-      <c r="AB105" s="12"/>
-      <c r="AC105" s="12"/>
-      <c r="AD105" s="12"/>
-      <c r="AE105" s="12"/>
-      <c r="AF105" s="12"/>
-      <c r="AG105" s="12"/>
-      <c r="AH105" s="13"/>
+      <c r="AH105" s="6"/>
     </row>
     <row r="106" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A106">
@@ -13614,13 +13471,7 @@
       <c r="AA106" t="s">
         <v>36</v>
       </c>
-      <c r="AB106" s="12"/>
-      <c r="AC106" s="12"/>
-      <c r="AD106" s="12"/>
-      <c r="AE106" s="12"/>
-      <c r="AF106" s="12"/>
-      <c r="AG106" s="12"/>
-      <c r="AH106" s="13"/>
+      <c r="AH106" s="6"/>
     </row>
     <row r="107" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A107">
@@ -13800,19 +13651,16 @@
       <c r="AA108" t="s">
         <v>36</v>
       </c>
-      <c r="AB108" s="12"/>
-      <c r="AC108" s="12"/>
-      <c r="AD108" s="12">
+      <c r="AD108">
         <v>1050</v>
       </c>
-      <c r="AE108" s="12">
+      <c r="AE108">
         <v>1</v>
       </c>
-      <c r="AF108" s="12">
+      <c r="AF108">
         <v>1</v>
       </c>
-      <c r="AG108" s="12"/>
-      <c r="AH108" s="13"/>
+      <c r="AH108" s="6"/>
     </row>
     <row r="109" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A109">
@@ -13897,13 +13745,7 @@
       <c r="AA109" t="s">
         <v>36</v>
       </c>
-      <c r="AB109" s="12"/>
-      <c r="AC109" s="12"/>
-      <c r="AD109" s="12"/>
-      <c r="AE109" s="12"/>
-      <c r="AF109" s="12"/>
-      <c r="AG109" s="12"/>
-      <c r="AH109" s="13"/>
+      <c r="AH109" s="6"/>
     </row>
     <row r="110" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A110">
@@ -13988,13 +13830,7 @@
       <c r="AA110" t="s">
         <v>36</v>
       </c>
-      <c r="AB110" s="12"/>
-      <c r="AC110" s="12"/>
-      <c r="AD110" s="12"/>
-      <c r="AE110" s="12"/>
-      <c r="AF110" s="12"/>
-      <c r="AG110" s="12"/>
-      <c r="AH110" s="13"/>
+      <c r="AH110" s="6"/>
     </row>
     <row r="111" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A111">
@@ -14079,15 +13915,10 @@
       <c r="AA111" t="s">
         <v>36</v>
       </c>
-      <c r="AB111" s="12"/>
-      <c r="AC111" s="12"/>
-      <c r="AD111" s="12">
+      <c r="AD111">
         <v>1225</v>
       </c>
-      <c r="AE111" s="12"/>
-      <c r="AF111" s="12"/>
-      <c r="AG111" s="12"/>
-      <c r="AH111" s="13"/>
+      <c r="AH111" s="6"/>
     </row>
     <row r="112" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A112">
@@ -14267,13 +14098,7 @@
       <c r="AA113" t="s">
         <v>36</v>
       </c>
-      <c r="AB113" s="12"/>
-      <c r="AC113" s="12"/>
-      <c r="AD113" s="12"/>
-      <c r="AE113" s="12"/>
-      <c r="AF113" s="12"/>
-      <c r="AG113" s="12"/>
-      <c r="AH113" s="13"/>
+      <c r="AH113" s="6"/>
     </row>
     <row r="114" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A114">
@@ -14453,13 +14278,7 @@
       <c r="AA115" t="s">
         <v>36</v>
       </c>
-      <c r="AB115" s="12"/>
-      <c r="AC115" s="12"/>
-      <c r="AD115" s="12"/>
-      <c r="AE115" s="12"/>
-      <c r="AF115" s="12"/>
-      <c r="AG115" s="12"/>
-      <c r="AH115" s="13"/>
+      <c r="AH115" s="6"/>
     </row>
     <row r="116" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A116">
@@ -14544,13 +14363,7 @@
       <c r="AA116" t="s">
         <v>36</v>
       </c>
-      <c r="AB116" s="12"/>
-      <c r="AC116" s="12"/>
-      <c r="AD116" s="12"/>
-      <c r="AE116" s="12"/>
-      <c r="AF116" s="12"/>
-      <c r="AG116" s="12"/>
-      <c r="AH116" s="13"/>
+      <c r="AH116" s="6"/>
     </row>
     <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117">
@@ -14635,13 +14448,7 @@
       <c r="AA117" t="s">
         <v>36</v>
       </c>
-      <c r="AB117" s="12"/>
-      <c r="AC117" s="12"/>
-      <c r="AD117" s="12"/>
-      <c r="AE117" s="12"/>
-      <c r="AF117" s="12"/>
-      <c r="AG117" s="12"/>
-      <c r="AH117" s="13"/>
+      <c r="AH117" s="6"/>
     </row>
     <row r="118" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A118">
@@ -14726,15 +14533,10 @@
       <c r="AA118" t="s">
         <v>36</v>
       </c>
-      <c r="AB118" s="12"/>
-      <c r="AC118" s="12"/>
-      <c r="AD118" s="12">
+      <c r="AD118">
         <v>1876</v>
       </c>
-      <c r="AE118" s="12"/>
-      <c r="AF118" s="12"/>
-      <c r="AG118" s="12"/>
-      <c r="AH118" s="13"/>
+      <c r="AH118" s="6"/>
     </row>
     <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119">
@@ -14819,19 +14621,16 @@
       <c r="AA119" t="s">
         <v>36</v>
       </c>
-      <c r="AB119" s="12"/>
-      <c r="AC119" s="12"/>
-      <c r="AD119" s="12">
+      <c r="AD119">
         <v>1470</v>
       </c>
-      <c r="AE119" s="12">
+      <c r="AE119">
         <v>1</v>
       </c>
-      <c r="AF119" s="12">
+      <c r="AF119">
         <v>1</v>
       </c>
-      <c r="AG119" s="12"/>
-      <c r="AH119" s="13"/>
+      <c r="AH119" s="6"/>
     </row>
     <row r="120" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A120">
@@ -14916,13 +14715,7 @@
       <c r="AA120" t="s">
         <v>36</v>
       </c>
-      <c r="AB120" s="12"/>
-      <c r="AC120" s="12"/>
-      <c r="AD120" s="12"/>
-      <c r="AE120" s="12"/>
-      <c r="AF120" s="12"/>
-      <c r="AG120" s="12"/>
-      <c r="AH120" s="13"/>
+      <c r="AH120" s="6"/>
     </row>
     <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121">
@@ -15102,13 +14895,7 @@
       <c r="AA122" t="s">
         <v>36</v>
       </c>
-      <c r="AB122" s="12"/>
-      <c r="AC122" s="12"/>
-      <c r="AD122" s="12"/>
-      <c r="AE122" s="12"/>
-      <c r="AF122" s="12"/>
-      <c r="AG122" s="12"/>
-      <c r="AH122" s="13"/>
+      <c r="AH122" s="6"/>
     </row>
     <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123">
@@ -15193,13 +14980,7 @@
       <c r="AA123" t="s">
         <v>36</v>
       </c>
-      <c r="AB123" s="12"/>
-      <c r="AC123" s="12"/>
-      <c r="AD123" s="12"/>
-      <c r="AE123" s="12"/>
-      <c r="AF123" s="12"/>
-      <c r="AG123" s="12"/>
-      <c r="AH123" s="13"/>
+      <c r="AH123" s="6"/>
     </row>
     <row r="124" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A124">
@@ -15284,13 +15065,7 @@
       <c r="AA124" t="s">
         <v>36</v>
       </c>
-      <c r="AB124" s="12"/>
-      <c r="AC124" s="12"/>
-      <c r="AD124" s="12"/>
-      <c r="AE124" s="12"/>
-      <c r="AF124" s="12"/>
-      <c r="AG124" s="12"/>
-      <c r="AH124" s="13"/>
+      <c r="AH124" s="6"/>
     </row>
     <row r="125" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A125">
@@ -15375,19 +15150,16 @@
       <c r="AA125" t="s">
         <v>36</v>
       </c>
-      <c r="AB125" s="12"/>
-      <c r="AC125" s="12"/>
-      <c r="AD125" s="12">
+      <c r="AD125">
         <v>840</v>
       </c>
-      <c r="AE125" s="12">
+      <c r="AE125">
         <v>1</v>
       </c>
-      <c r="AF125" s="12">
+      <c r="AF125">
         <v>1</v>
       </c>
-      <c r="AG125" s="12"/>
-      <c r="AH125" s="13"/>
+      <c r="AH125" s="6"/>
     </row>
     <row r="126" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A126">
@@ -15472,13 +15244,7 @@
       <c r="AA126" t="s">
         <v>36</v>
       </c>
-      <c r="AB126" s="12"/>
-      <c r="AC126" s="12"/>
-      <c r="AD126" s="12"/>
-      <c r="AE126" s="12"/>
-      <c r="AF126" s="12"/>
-      <c r="AG126" s="12"/>
-      <c r="AH126" s="13"/>
+      <c r="AH126" s="6"/>
     </row>
     <row r="127" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A127">
@@ -15563,15 +15329,10 @@
       <c r="AA127" t="s">
         <v>36</v>
       </c>
-      <c r="AB127" s="12"/>
-      <c r="AC127" s="12"/>
-      <c r="AD127" s="12"/>
-      <c r="AE127" s="12"/>
-      <c r="AF127" s="12">
+      <c r="AF127">
         <v>1</v>
       </c>
-      <c r="AG127" s="12"/>
-      <c r="AH127" s="13"/>
+      <c r="AH127" s="6"/>
     </row>
     <row r="128" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A128">
@@ -15656,13 +15417,7 @@
       <c r="AA128" t="s">
         <v>36</v>
       </c>
-      <c r="AB128" s="12"/>
-      <c r="AC128" s="12"/>
-      <c r="AD128" s="12"/>
-      <c r="AE128" s="12"/>
-      <c r="AF128" s="12"/>
-      <c r="AG128" s="12"/>
-      <c r="AH128" s="13"/>
+      <c r="AH128" s="6"/>
     </row>
     <row r="129" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A129">
@@ -15747,13 +15502,7 @@
       <c r="AA129" t="s">
         <v>36</v>
       </c>
-      <c r="AB129" s="12"/>
-      <c r="AC129" s="12"/>
-      <c r="AD129" s="12"/>
-      <c r="AE129" s="12"/>
-      <c r="AF129" s="12"/>
-      <c r="AG129" s="12"/>
-      <c r="AH129" s="13"/>
+      <c r="AH129" s="6"/>
     </row>
     <row r="130" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A130">
@@ -15933,13 +15682,7 @@
       <c r="AA131" t="s">
         <v>36</v>
       </c>
-      <c r="AB131" s="12"/>
-      <c r="AC131" s="12"/>
-      <c r="AD131" s="12"/>
-      <c r="AE131" s="12"/>
-      <c r="AF131" s="12"/>
-      <c r="AG131" s="12"/>
-      <c r="AH131" s="13"/>
+      <c r="AH131" s="6"/>
     </row>
     <row r="132" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A132">
@@ -16024,13 +15767,7 @@
       <c r="AA132" t="s">
         <v>36</v>
       </c>
-      <c r="AB132" s="12"/>
-      <c r="AC132" s="12"/>
-      <c r="AD132" s="12"/>
-      <c r="AE132" s="12"/>
-      <c r="AF132" s="12"/>
-      <c r="AG132" s="12"/>
-      <c r="AH132" s="13"/>
+      <c r="AH132" s="6"/>
     </row>
     <row r="133" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A133">
@@ -16115,13 +15852,7 @@
       <c r="AA133" t="s">
         <v>36</v>
       </c>
-      <c r="AB133" s="12"/>
-      <c r="AC133" s="12"/>
-      <c r="AD133" s="12"/>
-      <c r="AE133" s="12"/>
-      <c r="AF133" s="12"/>
-      <c r="AG133" s="12"/>
-      <c r="AH133" s="13"/>
+      <c r="AH133" s="6"/>
     </row>
     <row r="134" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A134">
@@ -16481,13 +16212,7 @@
       <c r="AA137" t="s">
         <v>36</v>
       </c>
-      <c r="AB137" s="12"/>
-      <c r="AC137" s="12"/>
-      <c r="AD137" s="12"/>
-      <c r="AE137" s="12"/>
-      <c r="AF137" s="12"/>
-      <c r="AG137" s="12"/>
-      <c r="AH137" s="13"/>
+      <c r="AH137" s="6"/>
     </row>
     <row r="138" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A138">
@@ -16847,13 +16572,7 @@
       <c r="AA141" t="s">
         <v>36</v>
       </c>
-      <c r="AB141" s="12"/>
-      <c r="AC141" s="12"/>
-      <c r="AD141" s="12"/>
-      <c r="AE141" s="12"/>
-      <c r="AF141" s="12"/>
-      <c r="AG141" s="12"/>
-      <c r="AH141" s="13"/>
+      <c r="AH141" s="6"/>
     </row>
     <row r="142" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A142">
@@ -16938,13 +16657,7 @@
       <c r="AA142" t="s">
         <v>36</v>
       </c>
-      <c r="AB142" s="12"/>
-      <c r="AC142" s="12"/>
-      <c r="AD142" s="12"/>
-      <c r="AE142" s="12"/>
-      <c r="AF142" s="12"/>
-      <c r="AG142" s="12"/>
-      <c r="AH142" s="13"/>
+      <c r="AH142" s="6"/>
     </row>
     <row r="143" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A143">
@@ -17029,13 +16742,7 @@
       <c r="AA143" t="s">
         <v>36</v>
       </c>
-      <c r="AB143" s="12"/>
-      <c r="AC143" s="12"/>
-      <c r="AD143" s="12"/>
-      <c r="AE143" s="12"/>
-      <c r="AF143" s="12"/>
-      <c r="AG143" s="12"/>
-      <c r="AH143" s="13"/>
+      <c r="AH143" s="6"/>
     </row>
     <row r="144" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A144">
@@ -17120,13 +16827,7 @@
       <c r="AA144" t="s">
         <v>36</v>
       </c>
-      <c r="AB144" s="12"/>
-      <c r="AC144" s="12"/>
-      <c r="AD144" s="12"/>
-      <c r="AE144" s="12"/>
-      <c r="AF144" s="12"/>
-      <c r="AG144" s="12"/>
-      <c r="AH144" s="13"/>
+      <c r="AH144" s="6"/>
     </row>
     <row r="145" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A145">
@@ -17211,13 +16912,7 @@
       <c r="AA145" t="s">
         <v>36</v>
       </c>
-      <c r="AB145" s="12"/>
-      <c r="AC145" s="12"/>
-      <c r="AD145" s="12"/>
-      <c r="AE145" s="12"/>
-      <c r="AF145" s="12"/>
-      <c r="AG145" s="12"/>
-      <c r="AH145" s="13"/>
+      <c r="AH145" s="6"/>
     </row>
     <row r="146" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A146">
@@ -17302,13 +16997,7 @@
       <c r="AA146" t="s">
         <v>36</v>
       </c>
-      <c r="AB146" s="12"/>
-      <c r="AC146" s="12"/>
-      <c r="AD146" s="12"/>
-      <c r="AE146" s="12"/>
-      <c r="AF146" s="12"/>
-      <c r="AG146" s="12"/>
-      <c r="AH146" s="13"/>
+      <c r="AH146" s="6"/>
     </row>
     <row r="147" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A147">
@@ -17393,17 +17082,13 @@
       <c r="AA147" t="s">
         <v>36</v>
       </c>
-      <c r="AB147" s="12"/>
-      <c r="AC147" s="12"/>
-      <c r="AD147" s="12">
+      <c r="AD147">
         <v>865</v>
       </c>
-      <c r="AE147" s="12">
+      <c r="AE147">
         <v>1</v>
       </c>
-      <c r="AF147" s="12"/>
-      <c r="AG147" s="12"/>
-      <c r="AH147" s="13"/>
+      <c r="AH147" s="6"/>
     </row>
     <row r="148" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A148">
@@ -17488,13 +17173,7 @@
       <c r="AA148" t="s">
         <v>36</v>
       </c>
-      <c r="AB148" s="12"/>
-      <c r="AC148" s="12"/>
-      <c r="AD148" s="12"/>
-      <c r="AE148" s="12"/>
-      <c r="AF148" s="12"/>
-      <c r="AG148" s="12"/>
-      <c r="AH148" s="13"/>
+      <c r="AH148" s="6"/>
     </row>
     <row r="149" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A149">
@@ -17579,13 +17258,7 @@
       <c r="AA149" t="s">
         <v>36</v>
       </c>
-      <c r="AB149" s="12"/>
-      <c r="AC149" s="12"/>
-      <c r="AD149" s="12"/>
-      <c r="AE149" s="12"/>
-      <c r="AF149" s="12"/>
-      <c r="AG149" s="12"/>
-      <c r="AH149" s="13"/>
+      <c r="AH149" s="6"/>
     </row>
     <row r="150" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A150">
@@ -17670,13 +17343,7 @@
       <c r="AA150" t="s">
         <v>36</v>
       </c>
-      <c r="AB150" s="12"/>
-      <c r="AC150" s="12"/>
-      <c r="AD150" s="12"/>
-      <c r="AE150" s="12"/>
-      <c r="AF150" s="12"/>
-      <c r="AG150" s="12"/>
-      <c r="AH150" s="13"/>
+      <c r="AH150" s="6"/>
     </row>
     <row r="151" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A151">
@@ -17761,13 +17428,7 @@
       <c r="AA151" t="s">
         <v>36</v>
       </c>
-      <c r="AB151" s="12"/>
-      <c r="AC151" s="12"/>
-      <c r="AD151" s="12"/>
-      <c r="AE151" s="12"/>
-      <c r="AF151" s="12"/>
-      <c r="AG151" s="12"/>
-      <c r="AH151" s="13"/>
+      <c r="AH151" s="6"/>
     </row>
     <row r="152" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A152">
@@ -17852,15 +17513,10 @@
       <c r="AA152" t="s">
         <v>36</v>
       </c>
-      <c r="AB152" s="12"/>
-      <c r="AC152" s="12"/>
-      <c r="AD152" s="12">
+      <c r="AD152">
         <v>840</v>
       </c>
-      <c r="AE152" s="12"/>
-      <c r="AF152" s="12"/>
-      <c r="AG152" s="12"/>
-      <c r="AH152" s="13"/>
+      <c r="AH152" s="6"/>
     </row>
     <row r="153" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A153">
@@ -18125,13 +17781,7 @@
       <c r="AA155" t="s">
         <v>36</v>
       </c>
-      <c r="AB155" s="12"/>
-      <c r="AC155" s="12"/>
-      <c r="AD155" s="12"/>
-      <c r="AE155" s="12"/>
-      <c r="AF155" s="12"/>
-      <c r="AG155" s="12"/>
-      <c r="AH155" s="13"/>
+      <c r="AH155" s="6"/>
     </row>
     <row r="156" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A156">
@@ -18585,13 +18235,7 @@
       <c r="AA160" t="s">
         <v>36</v>
       </c>
-      <c r="AB160" s="12"/>
-      <c r="AC160" s="12"/>
-      <c r="AD160" s="12"/>
-      <c r="AE160" s="12"/>
-      <c r="AF160" s="12"/>
-      <c r="AG160" s="12"/>
-      <c r="AH160" s="13"/>
+      <c r="AH160" s="6"/>
     </row>
     <row r="161" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A161">
@@ -18676,13 +18320,7 @@
       <c r="AA161" t="s">
         <v>36</v>
       </c>
-      <c r="AB161" s="12"/>
-      <c r="AC161" s="12"/>
-      <c r="AD161" s="12"/>
-      <c r="AE161" s="12"/>
-      <c r="AF161" s="12"/>
-      <c r="AG161" s="12"/>
-      <c r="AH161" s="13"/>
+      <c r="AH161" s="6"/>
     </row>
     <row r="162" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A162">
@@ -18767,17 +18405,13 @@
       <c r="AA162" t="s">
         <v>36</v>
       </c>
-      <c r="AB162" s="12"/>
-      <c r="AC162" s="12"/>
-      <c r="AD162" s="12"/>
-      <c r="AE162" s="12">
+      <c r="AE162">
         <v>1</v>
       </c>
-      <c r="AF162" s="12">
+      <c r="AF162">
         <v>2</v>
       </c>
-      <c r="AG162" s="12"/>
-      <c r="AH162" s="13"/>
+      <c r="AH162" s="6"/>
     </row>
     <row r="163" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A163">
@@ -18862,19 +18496,16 @@
       <c r="AA163" t="s">
         <v>36</v>
       </c>
-      <c r="AB163" s="12"/>
-      <c r="AC163" s="12"/>
-      <c r="AD163" s="12">
+      <c r="AD163">
         <v>820</v>
       </c>
-      <c r="AE163" s="12">
+      <c r="AE163">
         <v>1</v>
       </c>
-      <c r="AF163" s="12">
+      <c r="AF163">
         <v>1</v>
       </c>
-      <c r="AG163" s="12"/>
-      <c r="AH163" s="13"/>
+      <c r="AH163" s="6"/>
     </row>
     <row r="164" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A164">
@@ -19054,13 +18685,7 @@
       <c r="AA165" t="s">
         <v>36</v>
       </c>
-      <c r="AB165" s="12"/>
-      <c r="AC165" s="12"/>
-      <c r="AD165" s="12"/>
-      <c r="AE165" s="12"/>
-      <c r="AF165" s="12"/>
-      <c r="AG165" s="12"/>
-      <c r="AH165" s="13"/>
+      <c r="AH165" s="6"/>
     </row>
     <row r="166" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A166">
@@ -19145,13 +18770,7 @@
       <c r="AA166" t="s">
         <v>36</v>
       </c>
-      <c r="AB166" s="12"/>
-      <c r="AC166" s="12"/>
-      <c r="AD166" s="12"/>
-      <c r="AE166" s="12"/>
-      <c r="AF166" s="12"/>
-      <c r="AG166" s="12"/>
-      <c r="AH166" s="13"/>
+      <c r="AH166" s="6"/>
     </row>
     <row r="167" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A167">
@@ -19236,19 +18855,16 @@
       <c r="AA167" t="s">
         <v>36</v>
       </c>
-      <c r="AB167" s="12"/>
-      <c r="AC167" s="12"/>
-      <c r="AD167" s="12">
+      <c r="AD167">
         <v>1650</v>
       </c>
-      <c r="AE167" s="12">
+      <c r="AE167">
         <v>1</v>
       </c>
-      <c r="AF167" s="12">
+      <c r="AF167">
         <v>1</v>
       </c>
-      <c r="AG167" s="12"/>
-      <c r="AH167" s="13"/>
+      <c r="AH167" s="6"/>
     </row>
     <row r="168" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A168">
@@ -19333,17 +18949,13 @@
       <c r="AA168" t="s">
         <v>36</v>
       </c>
-      <c r="AB168" s="12"/>
-      <c r="AC168" s="12"/>
-      <c r="AD168" s="12"/>
-      <c r="AE168" s="12">
+      <c r="AE168">
         <v>1</v>
       </c>
-      <c r="AF168" s="12">
+      <c r="AF168">
         <v>1</v>
       </c>
-      <c r="AG168" s="12"/>
-      <c r="AH168" s="13"/>
+      <c r="AH168" s="6"/>
     </row>
     <row r="169" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A169">
@@ -19428,13 +19040,7 @@
       <c r="AA169" t="s">
         <v>36</v>
       </c>
-      <c r="AB169" s="12"/>
-      <c r="AC169" s="12"/>
-      <c r="AD169" s="12"/>
-      <c r="AE169" s="12"/>
-      <c r="AF169" s="12"/>
-      <c r="AG169" s="12"/>
-      <c r="AH169" s="13"/>
+      <c r="AH169" s="6"/>
     </row>
     <row r="170" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A170">
@@ -19519,17 +19125,13 @@
       <c r="AA170" t="s">
         <v>36</v>
       </c>
-      <c r="AB170" s="12"/>
-      <c r="AC170" s="12"/>
-      <c r="AD170" s="12"/>
-      <c r="AE170" s="12">
+      <c r="AE170">
         <v>1</v>
       </c>
-      <c r="AF170" s="12">
+      <c r="AF170">
         <v>1</v>
       </c>
-      <c r="AG170" s="12"/>
-      <c r="AH170" s="13"/>
+      <c r="AH170" s="6"/>
     </row>
     <row r="171" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A171">
@@ -19614,13 +19216,7 @@
       <c r="AA171" t="s">
         <v>36</v>
       </c>
-      <c r="AB171" s="12"/>
-      <c r="AC171" s="12"/>
-      <c r="AD171" s="12"/>
-      <c r="AE171" s="12"/>
-      <c r="AF171" s="12"/>
-      <c r="AG171" s="12"/>
-      <c r="AH171" s="13"/>
+      <c r="AH171" s="6"/>
     </row>
     <row r="172" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A172">
@@ -19705,13 +19301,7 @@
       <c r="AA172" t="s">
         <v>36</v>
       </c>
-      <c r="AB172" s="12"/>
-      <c r="AC172" s="12"/>
-      <c r="AD172" s="12"/>
-      <c r="AE172" s="12"/>
-      <c r="AF172" s="12"/>
-      <c r="AG172" s="12"/>
-      <c r="AH172" s="13"/>
+      <c r="AH172" s="6"/>
     </row>
     <row r="173" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A173">
@@ -19796,13 +19386,7 @@
       <c r="AA173" t="s">
         <v>36</v>
       </c>
-      <c r="AB173" s="12"/>
-      <c r="AC173" s="12"/>
-      <c r="AD173" s="12"/>
-      <c r="AE173" s="12"/>
-      <c r="AF173" s="12"/>
-      <c r="AG173" s="12"/>
-      <c r="AH173" s="13"/>
+      <c r="AH173" s="6"/>
     </row>
     <row r="174" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A174">
@@ -19887,19 +19471,16 @@
       <c r="AA174" t="s">
         <v>36</v>
       </c>
-      <c r="AB174" s="12">
+      <c r="AB174">
         <v>10.624243999999999</v>
       </c>
-      <c r="AC174" s="12">
+      <c r="AC174">
         <v>46.848776999999998</v>
       </c>
-      <c r="AD174" s="12">
+      <c r="AD174">
         <v>2475</v>
       </c>
-      <c r="AE174" s="12"/>
-      <c r="AF174" s="12"/>
-      <c r="AG174" s="12"/>
-      <c r="AH174" s="13"/>
+      <c r="AH174" s="6"/>
     </row>
     <row r="175" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A175">
@@ -19984,17 +19565,13 @@
       <c r="AA175" t="s">
         <v>36</v>
       </c>
-      <c r="AB175" s="12"/>
-      <c r="AC175" s="12"/>
-      <c r="AD175" s="12"/>
-      <c r="AE175" s="12">
+      <c r="AE175">
         <v>1</v>
       </c>
-      <c r="AF175" s="12">
+      <c r="AF175">
         <v>2</v>
       </c>
-      <c r="AG175" s="12"/>
-      <c r="AH175" s="13"/>
+      <c r="AH175" s="6"/>
     </row>
     <row r="176" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A176">
@@ -20079,13 +19656,7 @@
       <c r="AA176" t="s">
         <v>36</v>
       </c>
-      <c r="AB176" s="12"/>
-      <c r="AC176" s="12"/>
-      <c r="AD176" s="12"/>
-      <c r="AE176" s="12"/>
-      <c r="AF176" s="12"/>
-      <c r="AG176" s="12"/>
-      <c r="AH176" s="13"/>
+      <c r="AH176" s="6"/>
     </row>
     <row r="177" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A177">
@@ -20265,13 +19836,7 @@
       <c r="AA178" t="s">
         <v>36</v>
       </c>
-      <c r="AB178" s="12"/>
-      <c r="AC178" s="12"/>
-      <c r="AD178" s="12"/>
-      <c r="AE178" s="12"/>
-      <c r="AF178" s="12"/>
-      <c r="AG178" s="12"/>
-      <c r="AH178" s="13"/>
+      <c r="AH178" s="6"/>
     </row>
     <row r="179" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A179">
@@ -20356,13 +19921,7 @@
       <c r="AA179" t="s">
         <v>36</v>
       </c>
-      <c r="AB179" s="12"/>
-      <c r="AC179" s="12"/>
-      <c r="AD179" s="12"/>
-      <c r="AE179" s="12"/>
-      <c r="AF179" s="12"/>
-      <c r="AG179" s="12"/>
-      <c r="AH179" s="13"/>
+      <c r="AH179" s="6"/>
     </row>
     <row r="180" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A180">
@@ -20447,13 +20006,7 @@
       <c r="AA180" t="s">
         <v>36</v>
       </c>
-      <c r="AB180" s="12"/>
-      <c r="AC180" s="12"/>
-      <c r="AD180" s="12"/>
-      <c r="AE180" s="12"/>
-      <c r="AF180" s="12"/>
-      <c r="AG180" s="12"/>
-      <c r="AH180" s="13"/>
+      <c r="AH180" s="6"/>
     </row>
     <row r="181" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A181">
@@ -20538,13 +20091,7 @@
       <c r="AA181" t="s">
         <v>36</v>
       </c>
-      <c r="AB181" s="12"/>
-      <c r="AC181" s="12"/>
-      <c r="AD181" s="12"/>
-      <c r="AE181" s="12"/>
-      <c r="AF181" s="12"/>
-      <c r="AG181" s="12"/>
-      <c r="AH181" s="13"/>
+      <c r="AH181" s="6"/>
     </row>
     <row r="182" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A182">
@@ -20629,13 +20176,7 @@
       <c r="AA182" t="s">
         <v>36</v>
       </c>
-      <c r="AB182" s="12"/>
-      <c r="AC182" s="12"/>
-      <c r="AD182" s="12"/>
-      <c r="AE182" s="12"/>
-      <c r="AF182" s="12"/>
-      <c r="AG182" s="12"/>
-      <c r="AH182" s="13"/>
+      <c r="AH182" s="6"/>
     </row>
     <row r="183" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A183">
@@ -20720,13 +20261,7 @@
       <c r="AA183" t="s">
         <v>36</v>
       </c>
-      <c r="AB183" s="12"/>
-      <c r="AC183" s="12"/>
-      <c r="AD183" s="12"/>
-      <c r="AE183" s="12"/>
-      <c r="AF183" s="12"/>
-      <c r="AG183" s="12"/>
-      <c r="AH183" s="13"/>
+      <c r="AH183" s="6"/>
     </row>
     <row r="184" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A184">
@@ -20811,13 +20346,7 @@
       <c r="AA184" t="s">
         <v>36</v>
       </c>
-      <c r="AB184" s="12"/>
-      <c r="AC184" s="12"/>
-      <c r="AD184" s="12"/>
-      <c r="AE184" s="12"/>
-      <c r="AF184" s="12"/>
-      <c r="AG184" s="12"/>
-      <c r="AH184" s="13"/>
+      <c r="AH184" s="6"/>
     </row>
     <row r="185" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A185">
@@ -20902,13 +20431,7 @@
       <c r="AA185" t="s">
         <v>36</v>
       </c>
-      <c r="AB185" s="12"/>
-      <c r="AC185" s="12"/>
-      <c r="AD185" s="12"/>
-      <c r="AE185" s="12"/>
-      <c r="AF185" s="12"/>
-      <c r="AG185" s="12"/>
-      <c r="AH185" s="13"/>
+      <c r="AH185" s="6"/>
     </row>
     <row r="186" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A186">
@@ -20993,13 +20516,7 @@
       <c r="AA186" t="s">
         <v>36</v>
       </c>
-      <c r="AB186" s="12"/>
-      <c r="AC186" s="12"/>
-      <c r="AD186" s="12"/>
-      <c r="AE186" s="12"/>
-      <c r="AF186" s="12"/>
-      <c r="AG186" s="12"/>
-      <c r="AH186" s="13"/>
+      <c r="AH186" s="6"/>
     </row>
     <row r="187" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A187">
@@ -21084,13 +20601,7 @@
       <c r="AA187" t="s">
         <v>36</v>
       </c>
-      <c r="AB187" s="12"/>
-      <c r="AC187" s="12"/>
-      <c r="AD187" s="12"/>
-      <c r="AE187" s="12"/>
-      <c r="AF187" s="12"/>
-      <c r="AG187" s="12"/>
-      <c r="AH187" s="13"/>
+      <c r="AH187" s="6"/>
     </row>
     <row r="188" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A188">
@@ -21175,13 +20686,7 @@
       <c r="AA188" t="s">
         <v>36</v>
       </c>
-      <c r="AB188" s="12"/>
-      <c r="AC188" s="12"/>
-      <c r="AD188" s="12"/>
-      <c r="AE188" s="12"/>
-      <c r="AF188" s="12"/>
-      <c r="AG188" s="12"/>
-      <c r="AH188" s="13"/>
+      <c r="AH188" s="6"/>
     </row>
     <row r="189" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A189">
@@ -21266,13 +20771,7 @@
       <c r="AA189" t="s">
         <v>36</v>
       </c>
-      <c r="AB189" s="12"/>
-      <c r="AC189" s="12"/>
-      <c r="AD189" s="12"/>
-      <c r="AE189" s="12"/>
-      <c r="AF189" s="12"/>
-      <c r="AG189" s="12"/>
-      <c r="AH189" s="13"/>
+      <c r="AH189" s="6"/>
     </row>
     <row r="190" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A190">
@@ -21357,15 +20856,10 @@
       <c r="AA190" t="s">
         <v>36</v>
       </c>
-      <c r="AB190" s="12"/>
-      <c r="AC190" s="12"/>
-      <c r="AD190" s="12">
+      <c r="AD190">
         <v>1879</v>
       </c>
-      <c r="AE190" s="12"/>
-      <c r="AF190" s="12"/>
-      <c r="AG190" s="12"/>
-      <c r="AH190" s="13"/>
+      <c r="AH190" s="6"/>
     </row>
     <row r="191" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A191">
@@ -21450,17 +20944,13 @@
       <c r="AA191" t="s">
         <v>36</v>
       </c>
-      <c r="AB191" s="12">
+      <c r="AB191">
         <v>11.114138000000001</v>
       </c>
-      <c r="AC191" s="12">
+      <c r="AC191">
         <v>46.828629999999997</v>
       </c>
-      <c r="AD191" s="12"/>
-      <c r="AE191" s="12"/>
-      <c r="AF191" s="12"/>
-      <c r="AG191" s="12"/>
-      <c r="AH191" s="13"/>
+      <c r="AH191" s="6"/>
     </row>
     <row r="192" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A192">
@@ -21545,13 +21035,7 @@
       <c r="AA192" t="s">
         <v>36</v>
       </c>
-      <c r="AB192" s="12"/>
-      <c r="AC192" s="12"/>
-      <c r="AD192" s="12"/>
-      <c r="AE192" s="12"/>
-      <c r="AF192" s="12"/>
-      <c r="AG192" s="12"/>
-      <c r="AH192" s="13"/>
+      <c r="AH192" s="6"/>
     </row>
     <row r="193" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A193">
@@ -21645,9 +21129,7 @@
       <c r="AD193">
         <v>2262</v>
       </c>
-      <c r="AF193" s="12"/>
-      <c r="AG193" s="12"/>
-      <c r="AH193" s="13" t="s">
+      <c r="AH193" s="6" t="s">
         <v>1172</v>
       </c>
     </row>
@@ -21734,13 +21216,10 @@
       <c r="AA194" t="s">
         <v>36</v>
       </c>
-      <c r="AD194" s="14">
+      <c r="AD194" s="12">
         <v>1624</v>
       </c>
-      <c r="AE194" s="12"/>
-      <c r="AF194" s="12"/>
-      <c r="AG194" s="12"/>
-      <c r="AH194" s="13" t="s">
+      <c r="AH194" s="6" t="s">
         <v>1172</v>
       </c>
     </row>
@@ -21827,13 +21306,7 @@
       <c r="AA195" t="s">
         <v>36</v>
       </c>
-      <c r="AB195" s="12"/>
-      <c r="AC195" s="12"/>
-      <c r="AD195" s="12"/>
-      <c r="AE195" s="12"/>
-      <c r="AF195" s="12"/>
-      <c r="AG195" s="12"/>
-      <c r="AH195" s="13"/>
+      <c r="AH195" s="6"/>
     </row>
     <row r="196" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A196">
@@ -21918,15 +21391,10 @@
       <c r="AA196" t="s">
         <v>36</v>
       </c>
-      <c r="AB196" s="12"/>
-      <c r="AC196" s="12"/>
-      <c r="AD196" s="12">
+      <c r="AD196">
         <v>568</v>
       </c>
-      <c r="AE196" s="12"/>
-      <c r="AF196" s="12"/>
-      <c r="AG196" s="12"/>
-      <c r="AH196" s="13" t="s">
+      <c r="AH196" s="6" t="s">
         <v>1173</v>
       </c>
     </row>
@@ -22013,13 +21481,7 @@
       <c r="AA197" t="s">
         <v>36</v>
       </c>
-      <c r="AB197" s="12"/>
-      <c r="AC197" s="12"/>
-      <c r="AD197" s="12"/>
-      <c r="AE197" s="12"/>
-      <c r="AF197" s="12"/>
-      <c r="AG197" s="12"/>
-      <c r="AH197" s="13"/>
+      <c r="AH197" s="6"/>
     </row>
     <row r="198" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A198">
@@ -22104,13 +21566,7 @@
       <c r="AA198" t="s">
         <v>36</v>
       </c>
-      <c r="AB198" s="12"/>
-      <c r="AC198" s="12"/>
-      <c r="AD198" s="12"/>
-      <c r="AE198" s="12"/>
-      <c r="AF198" s="12"/>
-      <c r="AG198" s="12"/>
-      <c r="AH198" s="13"/>
+      <c r="AH198" s="6"/>
     </row>
     <row r="199" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A199">
@@ -22195,13 +21651,7 @@
       <c r="AA199" t="s">
         <v>36</v>
       </c>
-      <c r="AB199" s="12"/>
-      <c r="AC199" s="12"/>
-      <c r="AD199" s="12"/>
-      <c r="AE199" s="12"/>
-      <c r="AF199" s="12"/>
-      <c r="AG199" s="12"/>
-      <c r="AH199" s="13"/>
+      <c r="AH199" s="6"/>
     </row>
     <row r="200" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A200">
@@ -22286,13 +21736,7 @@
       <c r="AA200" t="s">
         <v>36</v>
       </c>
-      <c r="AB200" s="12"/>
-      <c r="AC200" s="12"/>
-      <c r="AD200" s="12"/>
-      <c r="AE200" s="12"/>
-      <c r="AF200" s="12"/>
-      <c r="AG200" s="12"/>
-      <c r="AH200" s="13"/>
+      <c r="AH200" s="6"/>
     </row>
     <row r="201" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A201">
@@ -22377,13 +21821,7 @@
       <c r="AA201" t="s">
         <v>36</v>
       </c>
-      <c r="AB201" s="12"/>
-      <c r="AC201" s="12"/>
-      <c r="AD201" s="12"/>
-      <c r="AE201" s="12"/>
-      <c r="AF201" s="12"/>
-      <c r="AG201" s="12"/>
-      <c r="AH201" s="13"/>
+      <c r="AH201" s="6"/>
     </row>
     <row r="202" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A202">
@@ -22468,13 +21906,7 @@
       <c r="AA202" t="s">
         <v>36</v>
       </c>
-      <c r="AB202" s="12"/>
-      <c r="AC202" s="12"/>
-      <c r="AD202" s="12"/>
-      <c r="AE202" s="12"/>
-      <c r="AF202" s="12"/>
-      <c r="AG202" s="12"/>
-      <c r="AH202" s="13"/>
+      <c r="AH202" s="6"/>
     </row>
     <row r="203" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A203">
@@ -22559,13 +21991,7 @@
       <c r="AA203" t="s">
         <v>36</v>
       </c>
-      <c r="AB203" s="12"/>
-      <c r="AC203" s="12"/>
-      <c r="AD203" s="12"/>
-      <c r="AE203" s="12"/>
-      <c r="AF203" s="12"/>
-      <c r="AG203" s="12"/>
-      <c r="AH203" s="13"/>
+      <c r="AH203" s="6"/>
     </row>
     <row r="204" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A204">
@@ -22650,13 +22076,7 @@
       <c r="AA204" t="s">
         <v>36</v>
       </c>
-      <c r="AB204" s="12"/>
-      <c r="AC204" s="12"/>
-      <c r="AD204" s="12"/>
-      <c r="AE204" s="12"/>
-      <c r="AF204" s="12"/>
-      <c r="AG204" s="12"/>
-      <c r="AH204" s="13"/>
+      <c r="AH204" s="6"/>
     </row>
     <row r="205" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A205">
@@ -22741,19 +22161,16 @@
       <c r="AA205" t="s">
         <v>36</v>
       </c>
-      <c r="AB205" s="12"/>
-      <c r="AC205" s="12"/>
-      <c r="AD205" s="12">
+      <c r="AD205">
         <v>1240</v>
       </c>
-      <c r="AE205" s="12">
+      <c r="AE205">
         <v>1</v>
       </c>
-      <c r="AF205" s="12">
+      <c r="AF205">
         <v>1</v>
       </c>
-      <c r="AG205" s="12"/>
-      <c r="AH205" s="13"/>
+      <c r="AH205" s="6"/>
     </row>
     <row r="206" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A206">
@@ -22838,13 +22255,7 @@
       <c r="AA206" t="s">
         <v>36</v>
       </c>
-      <c r="AB206" s="12"/>
-      <c r="AC206" s="12"/>
-      <c r="AD206" s="12"/>
-      <c r="AE206" s="12"/>
-      <c r="AF206" s="12"/>
-      <c r="AG206" s="12"/>
-      <c r="AH206" s="13"/>
+      <c r="AH206" s="6"/>
     </row>
     <row r="207" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A207">
@@ -23024,13 +22435,7 @@
       <c r="AA208" t="s">
         <v>36</v>
       </c>
-      <c r="AB208" s="12"/>
-      <c r="AC208" s="12"/>
-      <c r="AD208" s="12"/>
-      <c r="AE208" s="12"/>
-      <c r="AF208" s="12"/>
-      <c r="AG208" s="12"/>
-      <c r="AH208" s="13"/>
+      <c r="AH208" s="6"/>
     </row>
     <row r="209" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A209">
@@ -23115,17 +22520,13 @@
       <c r="AA209" t="s">
         <v>36</v>
       </c>
-      <c r="AB209" s="12"/>
-      <c r="AC209" s="12"/>
-      <c r="AD209" s="12"/>
-      <c r="AE209" s="12">
+      <c r="AE209">
         <v>1</v>
       </c>
-      <c r="AF209" s="12">
+      <c r="AF209">
         <v>1</v>
       </c>
-      <c r="AG209" s="12"/>
-      <c r="AH209" s="13"/>
+      <c r="AH209" s="6"/>
     </row>
     <row r="210" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A210">
@@ -23210,13 +22611,7 @@
       <c r="AA210" t="s">
         <v>36</v>
       </c>
-      <c r="AB210" s="12"/>
-      <c r="AC210" s="12"/>
-      <c r="AD210" s="12"/>
-      <c r="AE210" s="12"/>
-      <c r="AF210" s="12"/>
-      <c r="AG210" s="12"/>
-      <c r="AH210" s="13"/>
+      <c r="AH210" s="6"/>
     </row>
     <row r="211" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A211">
@@ -23301,13 +22696,7 @@
       <c r="AA211" t="s">
         <v>36</v>
       </c>
-      <c r="AB211" s="12"/>
-      <c r="AC211" s="12"/>
-      <c r="AD211" s="12"/>
-      <c r="AE211" s="12"/>
-      <c r="AF211" s="12"/>
-      <c r="AG211" s="12"/>
-      <c r="AH211" s="13"/>
+      <c r="AH211" s="6"/>
     </row>
     <row r="212" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A212">
@@ -23487,13 +22876,7 @@
       <c r="AA213" t="s">
         <v>36</v>
       </c>
-      <c r="AB213" s="12"/>
-      <c r="AC213" s="12"/>
-      <c r="AD213" s="12"/>
-      <c r="AE213" s="12"/>
-      <c r="AF213" s="12"/>
-      <c r="AG213" s="12"/>
-      <c r="AH213" s="13"/>
+      <c r="AH213" s="6"/>
     </row>
     <row r="214" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A214">
@@ -23578,13 +22961,7 @@
       <c r="AA214" t="s">
         <v>36</v>
       </c>
-      <c r="AB214" s="12"/>
-      <c r="AC214" s="12"/>
-      <c r="AD214" s="12"/>
-      <c r="AE214" s="12"/>
-      <c r="AF214" s="12"/>
-      <c r="AG214" s="12"/>
-      <c r="AH214" s="13"/>
+      <c r="AH214" s="6"/>
     </row>
     <row r="215" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A215">
@@ -23669,15 +23046,10 @@
       <c r="AA215" t="s">
         <v>36</v>
       </c>
-      <c r="AB215" s="12"/>
-      <c r="AC215" s="12"/>
-      <c r="AD215" s="12">
+      <c r="AD215">
         <v>1326</v>
       </c>
-      <c r="AE215" s="12"/>
-      <c r="AF215" s="12"/>
-      <c r="AG215" s="12"/>
-      <c r="AH215" s="13"/>
+      <c r="AH215" s="6"/>
     </row>
     <row r="216" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A216">
@@ -23762,13 +23134,7 @@
       <c r="AA216" t="s">
         <v>36</v>
       </c>
-      <c r="AB216" s="12"/>
-      <c r="AC216" s="12"/>
-      <c r="AD216" s="12"/>
-      <c r="AE216" s="12"/>
-      <c r="AF216" s="12"/>
-      <c r="AG216" s="12"/>
-      <c r="AH216" s="13"/>
+      <c r="AH216" s="6"/>
     </row>
     <row r="217" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A217">
@@ -23944,13 +23310,7 @@
       <c r="AA218" t="s">
         <v>36</v>
       </c>
-      <c r="AB218" s="12"/>
-      <c r="AC218" s="12"/>
-      <c r="AD218" s="12"/>
-      <c r="AE218" s="12"/>
-      <c r="AF218" s="12"/>
-      <c r="AG218" s="12"/>
-      <c r="AH218" s="13"/>
+      <c r="AH218" s="6"/>
     </row>
     <row r="219" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A219">
@@ -24035,13 +23395,7 @@
       <c r="AA219" t="s">
         <v>36</v>
       </c>
-      <c r="AB219" s="12"/>
-      <c r="AC219" s="12"/>
-      <c r="AD219" s="12"/>
-      <c r="AE219" s="12"/>
-      <c r="AF219" s="12"/>
-      <c r="AG219" s="12"/>
-      <c r="AH219" s="13"/>
+      <c r="AH219" s="6"/>
     </row>
     <row r="220" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A220">
@@ -24126,13 +23480,7 @@
       <c r="AA220" t="s">
         <v>36</v>
       </c>
-      <c r="AB220" s="12"/>
-      <c r="AC220" s="12"/>
-      <c r="AD220" s="12"/>
-      <c r="AE220" s="12"/>
-      <c r="AF220" s="12"/>
-      <c r="AG220" s="12"/>
-      <c r="AH220" s="13"/>
+      <c r="AH220" s="6"/>
     </row>
     <row r="221" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A221">
@@ -24217,13 +23565,7 @@
       <c r="AA221" t="s">
         <v>36</v>
       </c>
-      <c r="AB221" s="12"/>
-      <c r="AC221" s="12"/>
-      <c r="AD221" s="12"/>
-      <c r="AE221" s="12"/>
-      <c r="AF221" s="12"/>
-      <c r="AG221" s="12"/>
-      <c r="AH221" s="13"/>
+      <c r="AH221" s="6"/>
     </row>
     <row r="222" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A222">
@@ -24308,15 +23650,10 @@
       <c r="AA222" t="s">
         <v>36</v>
       </c>
-      <c r="AB222" s="12"/>
-      <c r="AC222" s="12"/>
-      <c r="AD222" s="12">
+      <c r="AD222">
         <v>1412</v>
       </c>
-      <c r="AE222" s="12"/>
-      <c r="AF222" s="12"/>
-      <c r="AG222" s="12"/>
-      <c r="AH222" s="13"/>
+      <c r="AH222" s="6"/>
     </row>
     <row r="223" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A223">
@@ -24401,13 +23738,7 @@
       <c r="AA223" t="s">
         <v>36</v>
       </c>
-      <c r="AB223" s="12"/>
-      <c r="AC223" s="12"/>
-      <c r="AD223" s="12"/>
-      <c r="AE223" s="12"/>
-      <c r="AF223" s="12"/>
-      <c r="AG223" s="12"/>
-      <c r="AH223" s="13"/>
+      <c r="AH223" s="6"/>
     </row>
     <row r="224" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A224">
@@ -24492,13 +23823,7 @@
       <c r="AA224" t="s">
         <v>36</v>
       </c>
-      <c r="AB224" s="12"/>
-      <c r="AC224" s="12"/>
-      <c r="AD224" s="12"/>
-      <c r="AE224" s="12"/>
-      <c r="AF224" s="12"/>
-      <c r="AG224" s="12"/>
-      <c r="AH224" s="13"/>
+      <c r="AH224" s="6"/>
     </row>
     <row r="225" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A225">
@@ -24678,13 +24003,7 @@
       <c r="AA226" t="s">
         <v>36</v>
       </c>
-      <c r="AB226" s="12"/>
-      <c r="AC226" s="12"/>
-      <c r="AD226" s="12"/>
-      <c r="AE226" s="12"/>
-      <c r="AF226" s="12"/>
-      <c r="AG226" s="12"/>
-      <c r="AH226" s="13"/>
+      <c r="AH226" s="6"/>
     </row>
     <row r="227" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A227">
@@ -24769,15 +24088,10 @@
       <c r="AA227" t="s">
         <v>36</v>
       </c>
-      <c r="AB227" s="12"/>
-      <c r="AC227" s="12"/>
-      <c r="AD227" s="12">
+      <c r="AD227">
         <v>2127</v>
       </c>
-      <c r="AE227" s="12"/>
-      <c r="AF227" s="12"/>
-      <c r="AG227" s="12"/>
-      <c r="AH227" s="13"/>
+      <c r="AH227" s="6"/>
     </row>
     <row r="228" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A228">
@@ -24862,15 +24176,10 @@
       <c r="AA228" t="s">
         <v>36</v>
       </c>
-      <c r="AB228" s="12"/>
-      <c r="AC228" s="12"/>
-      <c r="AD228" s="12">
+      <c r="AD228">
         <v>484</v>
       </c>
-      <c r="AE228" s="12"/>
-      <c r="AF228" s="12"/>
-      <c r="AG228" s="12"/>
-      <c r="AH228" s="13"/>
+      <c r="AH228" s="6"/>
     </row>
     <row r="229" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A229">
@@ -24955,13 +24264,7 @@
       <c r="AA229" t="s">
         <v>36</v>
       </c>
-      <c r="AB229" s="12"/>
-      <c r="AC229" s="12"/>
-      <c r="AD229" s="12"/>
-      <c r="AE229" s="12"/>
-      <c r="AF229" s="12"/>
-      <c r="AG229" s="12"/>
-      <c r="AH229" s="13"/>
+      <c r="AH229" s="6"/>
     </row>
     <row r="230" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A230">
@@ -25046,13 +24349,7 @@
       <c r="AA230" t="s">
         <v>36</v>
       </c>
-      <c r="AB230" s="12"/>
-      <c r="AC230" s="12"/>
-      <c r="AD230" s="12"/>
-      <c r="AE230" s="12"/>
-      <c r="AF230" s="12"/>
-      <c r="AG230" s="12"/>
-      <c r="AH230" s="13"/>
+      <c r="AH230" s="6"/>
     </row>
     <row r="231" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A231">
@@ -25137,13 +24434,7 @@
       <c r="AA231" t="s">
         <v>36</v>
       </c>
-      <c r="AB231" s="12"/>
-      <c r="AC231" s="12"/>
-      <c r="AD231" s="12"/>
-      <c r="AE231" s="12"/>
-      <c r="AF231" s="12"/>
-      <c r="AG231" s="12"/>
-      <c r="AH231" s="13"/>
+      <c r="AH231" s="6"/>
     </row>
     <row r="232" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A232">
@@ -25228,13 +24519,7 @@
       <c r="AA232" t="s">
         <v>36</v>
       </c>
-      <c r="AB232" s="12"/>
-      <c r="AC232" s="12"/>
-      <c r="AD232" s="12"/>
-      <c r="AE232" s="12"/>
-      <c r="AF232" s="12"/>
-      <c r="AG232" s="12"/>
-      <c r="AH232" s="13"/>
+      <c r="AH232" s="6"/>
     </row>
     <row r="233" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A233">
@@ -25319,13 +24604,7 @@
       <c r="AA233" t="s">
         <v>36</v>
       </c>
-      <c r="AB233" s="12"/>
-      <c r="AC233" s="12"/>
-      <c r="AD233" s="12"/>
-      <c r="AE233" s="12"/>
-      <c r="AF233" s="12"/>
-      <c r="AG233" s="12"/>
-      <c r="AH233" s="13"/>
+      <c r="AH233" s="6"/>
     </row>
     <row r="234" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A234">
@@ -25410,13 +24689,7 @@
       <c r="AA234" t="s">
         <v>36</v>
       </c>
-      <c r="AB234" s="12"/>
-      <c r="AC234" s="12"/>
-      <c r="AD234" s="12"/>
-      <c r="AE234" s="12"/>
-      <c r="AF234" s="12"/>
-      <c r="AG234" s="12"/>
-      <c r="AH234" s="13"/>
+      <c r="AH234" s="6"/>
     </row>
     <row r="235" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A235">
@@ -25501,13 +24774,7 @@
       <c r="AA235" t="s">
         <v>36</v>
       </c>
-      <c r="AB235" s="12"/>
-      <c r="AC235" s="12"/>
-      <c r="AD235" s="12"/>
-      <c r="AE235" s="12"/>
-      <c r="AF235" s="12"/>
-      <c r="AG235" s="12"/>
-      <c r="AH235" s="13"/>
+      <c r="AH235" s="6"/>
     </row>
     <row r="236" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A236">
@@ -25592,13 +24859,7 @@
       <c r="AA236" t="s">
         <v>36</v>
       </c>
-      <c r="AB236" s="12"/>
-      <c r="AC236" s="12"/>
-      <c r="AD236" s="12"/>
-      <c r="AE236" s="12"/>
-      <c r="AF236" s="12"/>
-      <c r="AG236" s="12"/>
-      <c r="AH236" s="13"/>
+      <c r="AH236" s="6"/>
     </row>
     <row r="237" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A237">
@@ -25683,13 +24944,7 @@
       <c r="AA237" t="s">
         <v>36</v>
       </c>
-      <c r="AB237" s="12"/>
-      <c r="AC237" s="12"/>
-      <c r="AD237" s="12"/>
-      <c r="AE237" s="12"/>
-      <c r="AF237" s="12"/>
-      <c r="AG237" s="12"/>
-      <c r="AH237" s="13"/>
+      <c r="AH237" s="6"/>
     </row>
     <row r="238" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A238">
@@ -25774,15 +25029,10 @@
       <c r="AA238" t="s">
         <v>36</v>
       </c>
-      <c r="AB238" s="12"/>
-      <c r="AC238" s="12"/>
-      <c r="AD238" s="12">
+      <c r="AD238">
         <v>1621</v>
       </c>
-      <c r="AE238" s="12"/>
-      <c r="AF238" s="12"/>
-      <c r="AG238" s="12"/>
-      <c r="AH238" s="13"/>
+      <c r="AH238" s="6"/>
     </row>
     <row r="239" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A239">
@@ -26138,13 +25388,7 @@
       <c r="AA242" t="s">
         <v>36</v>
       </c>
-      <c r="AB242" s="12"/>
-      <c r="AC242" s="12"/>
-      <c r="AD242" s="12"/>
-      <c r="AE242" s="12"/>
-      <c r="AF242" s="12"/>
-      <c r="AG242" s="12"/>
-      <c r="AH242" s="13"/>
+      <c r="AH242" s="6"/>
     </row>
     <row r="243" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A243">
@@ -26229,13 +25473,7 @@
       <c r="AA243" t="s">
         <v>36</v>
       </c>
-      <c r="AB243" s="12"/>
-      <c r="AC243" s="12"/>
-      <c r="AD243" s="12"/>
-      <c r="AE243" s="12"/>
-      <c r="AF243" s="12"/>
-      <c r="AG243" s="12"/>
-      <c r="AH243" s="13"/>
+      <c r="AH243" s="6"/>
     </row>
     <row r="244" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A244">
@@ -26320,13 +25558,7 @@
       <c r="AA244" t="s">
         <v>36</v>
       </c>
-      <c r="AB244" s="12"/>
-      <c r="AC244" s="12"/>
-      <c r="AD244" s="12"/>
-      <c r="AE244" s="12"/>
-      <c r="AF244" s="12"/>
-      <c r="AG244" s="12"/>
-      <c r="AH244" s="13"/>
+      <c r="AH244" s="6"/>
     </row>
     <row r="245" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A245">
@@ -26411,13 +25643,7 @@
       <c r="AA245" t="s">
         <v>36</v>
       </c>
-      <c r="AB245" s="12"/>
-      <c r="AC245" s="12"/>
-      <c r="AD245" s="12"/>
-      <c r="AE245" s="12"/>
-      <c r="AF245" s="12"/>
-      <c r="AG245" s="12"/>
-      <c r="AH245" s="13"/>
+      <c r="AH245" s="6"/>
     </row>
     <row r="246" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A246">
@@ -26502,13 +25728,7 @@
       <c r="AA246" t="s">
         <v>36</v>
       </c>
-      <c r="AB246" s="12"/>
-      <c r="AC246" s="12"/>
-      <c r="AD246" s="12"/>
-      <c r="AE246" s="12"/>
-      <c r="AF246" s="12"/>
-      <c r="AG246" s="12"/>
-      <c r="AH246" s="13"/>
+      <c r="AH246" s="6"/>
     </row>
     <row r="247" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A247">
@@ -26593,13 +25813,7 @@
       <c r="AA247" t="s">
         <v>36</v>
       </c>
-      <c r="AB247" s="12"/>
-      <c r="AC247" s="12"/>
-      <c r="AD247" s="12"/>
-      <c r="AE247" s="12"/>
-      <c r="AF247" s="12"/>
-      <c r="AG247" s="12"/>
-      <c r="AH247" s="13"/>
+      <c r="AH247" s="6"/>
     </row>
     <row r="248" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A248">
@@ -26684,13 +25898,7 @@
       <c r="AA248" t="s">
         <v>36</v>
       </c>
-      <c r="AB248" s="12"/>
-      <c r="AC248" s="12"/>
-      <c r="AD248" s="12"/>
-      <c r="AE248" s="12"/>
-      <c r="AF248" s="12"/>
-      <c r="AG248" s="12"/>
-      <c r="AH248" s="13"/>
+      <c r="AH248" s="6"/>
     </row>
     <row r="249" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A249">
@@ -26775,13 +25983,7 @@
       <c r="AA249" t="s">
         <v>36</v>
       </c>
-      <c r="AB249" s="12"/>
-      <c r="AC249" s="12"/>
-      <c r="AD249" s="12"/>
-      <c r="AE249" s="12"/>
-      <c r="AF249" s="12"/>
-      <c r="AG249" s="12"/>
-      <c r="AH249" s="13"/>
+      <c r="AH249" s="6"/>
     </row>
     <row r="250" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A250">
@@ -27060,13 +26262,7 @@
       <c r="AA252" t="s">
         <v>36</v>
       </c>
-      <c r="AB252" s="12"/>
-      <c r="AC252" s="12"/>
-      <c r="AD252" s="12"/>
-      <c r="AE252" s="12"/>
-      <c r="AF252" s="12"/>
-      <c r="AG252" s="12"/>
-      <c r="AH252" s="13"/>
+      <c r="AH252" s="6"/>
     </row>
     <row r="253" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A253">
@@ -27151,13 +26347,7 @@
       <c r="AA253" t="s">
         <v>36</v>
       </c>
-      <c r="AB253" s="12"/>
-      <c r="AC253" s="12"/>
-      <c r="AD253" s="12"/>
-      <c r="AE253" s="12"/>
-      <c r="AF253" s="12"/>
-      <c r="AG253" s="12"/>
-      <c r="AH253" s="13"/>
+      <c r="AH253" s="6"/>
     </row>
     <row r="254" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A254">
@@ -27242,13 +26432,7 @@
       <c r="AA254" t="s">
         <v>36</v>
       </c>
-      <c r="AB254" s="12"/>
-      <c r="AC254" s="12"/>
-      <c r="AD254" s="12"/>
-      <c r="AE254" s="12"/>
-      <c r="AF254" s="12"/>
-      <c r="AG254" s="12"/>
-      <c r="AH254" s="13"/>
+      <c r="AH254" s="6"/>
     </row>
     <row r="255" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A255">
@@ -27333,13 +26517,7 @@
       <c r="AA255" t="s">
         <v>36</v>
       </c>
-      <c r="AB255" s="12"/>
-      <c r="AC255" s="12"/>
-      <c r="AD255" s="12"/>
-      <c r="AE255" s="12"/>
-      <c r="AF255" s="12"/>
-      <c r="AG255" s="12"/>
-      <c r="AH255" s="13"/>
+      <c r="AH255" s="6"/>
     </row>
     <row r="256" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A256">
@@ -27424,13 +26602,7 @@
       <c r="AA256" t="s">
         <v>36</v>
       </c>
-      <c r="AB256" s="12"/>
-      <c r="AC256" s="12"/>
-      <c r="AD256" s="12"/>
-      <c r="AE256" s="12"/>
-      <c r="AF256" s="12"/>
-      <c r="AG256" s="12"/>
-      <c r="AH256" s="13"/>
+      <c r="AH256" s="6"/>
     </row>
     <row r="257" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A257">
@@ -27705,13 +26877,7 @@
       <c r="AA259" t="s">
         <v>36</v>
       </c>
-      <c r="AB259" s="12"/>
-      <c r="AC259" s="12"/>
-      <c r="AD259" s="12"/>
-      <c r="AE259" s="12"/>
-      <c r="AF259" s="12"/>
-      <c r="AG259" s="12"/>
-      <c r="AH259" s="13"/>
+      <c r="AH259" s="6"/>
     </row>
     <row r="260" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A260">
@@ -28071,13 +27237,7 @@
       <c r="AA263" t="s">
         <v>36</v>
       </c>
-      <c r="AB263" s="12"/>
-      <c r="AC263" s="12"/>
-      <c r="AD263" s="12"/>
-      <c r="AE263" s="12"/>
-      <c r="AF263" s="12"/>
-      <c r="AG263" s="12"/>
-      <c r="AH263" s="13"/>
+      <c r="AH263" s="6"/>
     </row>
     <row r="264" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A264">
@@ -28488,7 +27648,7 @@
       <c r="P268">
         <v>2577</v>
       </c>
-      <c r="Q268" s="12">
+      <c r="Q268">
         <v>2572.03344726562</v>
       </c>
       <c r="R268" t="s">
@@ -28573,7 +27733,7 @@
       <c r="P269">
         <v>1551</v>
       </c>
-      <c r="Q269" s="12">
+      <c r="Q269">
         <v>1543.84753417969</v>
       </c>
       <c r="R269" t="s">
@@ -28658,7 +27818,7 @@
       <c r="P270">
         <v>1800</v>
       </c>
-      <c r="Q270" s="12">
+      <c r="Q270">
         <v>1667.8818359375</v>
       </c>
       <c r="R270">
@@ -28692,10 +27852,10 @@
       <c r="AA270" t="s">
         <v>36</v>
       </c>
-      <c r="AB270" s="12">
+      <c r="AB270">
         <v>10.513056000000001</v>
       </c>
-      <c r="AC270" s="12">
+      <c r="AC270">
         <v>46.831667000000003</v>
       </c>
       <c r="AD270" s="7">
@@ -28791,8 +27951,6 @@
       <c r="AA271" t="s">
         <v>36</v>
       </c>
-      <c r="AB271" s="12"/>
-      <c r="AC271" s="12"/>
       <c r="AH271" s="6"/>
     </row>
     <row r="272" spans="1:34" x14ac:dyDescent="0.2">
@@ -30403,87 +29561,87 @@
       </c>
       <c r="AH289" s="6"/>
     </row>
-    <row r="290" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A290" s="12">
+    <row r="290" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A290">
         <v>531</v>
       </c>
-      <c r="B290" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C290" s="12">
+      <c r="B290" t="s">
+        <v>26</v>
+      </c>
+      <c r="C290">
         <v>2661</v>
       </c>
-      <c r="D290" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E290" s="12" t="s">
+      <c r="D290" t="s">
+        <v>26</v>
+      </c>
+      <c r="E290" t="s">
         <v>266</v>
       </c>
-      <c r="F290" s="12" t="s">
+      <c r="F290" t="s">
         <v>182</v>
       </c>
-      <c r="G290" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H290" s="12" t="s">
+      <c r="G290" t="s">
+        <v>26</v>
+      </c>
+      <c r="H290" t="s">
         <v>29</v>
       </c>
-      <c r="I290" s="12" t="s">
+      <c r="I290" t="s">
         <v>30</v>
       </c>
-      <c r="J290" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K290" s="12">
+      <c r="J290" t="s">
+        <v>31</v>
+      </c>
+      <c r="K290">
         <v>160080</v>
       </c>
-      <c r="L290" s="12">
+      <c r="L290">
         <v>2661</v>
       </c>
-      <c r="M290" s="12" t="s">
+      <c r="M290" t="s">
         <v>32</v>
       </c>
-      <c r="N290" s="12">
+      <c r="N290">
         <v>10.532999999999999</v>
       </c>
-      <c r="O290" s="12">
+      <c r="O290">
         <v>46.75</v>
       </c>
-      <c r="P290" s="12">
+      <c r="P290">
         <v>1461</v>
       </c>
-      <c r="Q290" s="12">
+      <c r="Q290">
         <v>1448</v>
       </c>
-      <c r="R290" s="12">
+      <c r="R290">
         <v>6686</v>
       </c>
-      <c r="S290" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="T290" s="12" t="s">
+      <c r="S290" t="s">
+        <v>34</v>
+      </c>
+      <c r="T290" t="s">
         <v>267</v>
       </c>
-      <c r="U290" s="12" t="s">
+      <c r="U290" t="s">
         <v>177</v>
       </c>
-      <c r="V290" s="15">
+      <c r="V290" s="1">
         <v>18629</v>
       </c>
-      <c r="W290" s="15">
+      <c r="W290" s="1">
         <v>45177</v>
       </c>
-      <c r="X290" s="12">
+      <c r="X290">
         <v>25837</v>
       </c>
-      <c r="Y290" s="16">
+      <c r="Y290" s="11">
         <f>Tabella2[[#This Row],[elevation]]-Tabella2[[#This Row],[elevation_glo30]]</f>
         <v>13</v>
       </c>
-      <c r="Z290" s="12">
+      <c r="Z290">
         <v>12241</v>
       </c>
-      <c r="AA290" s="12" t="s">
+      <c r="AA290" t="s">
         <v>36</v>
       </c>
       <c r="AB290">
@@ -30492,10 +29650,10 @@
       <c r="AC290">
         <v>46.759605999999998</v>
       </c>
-      <c r="AE290" s="12">
+      <c r="AE290">
         <v>1</v>
       </c>
-      <c r="AH290" s="13"/>
+      <c r="AH290" s="6"/>
     </row>
     <row r="291" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A291">
@@ -34623,13 +33781,7 @@
       <c r="AA337" t="s">
         <v>36</v>
       </c>
-      <c r="AB337" s="12"/>
-      <c r="AC337" s="12"/>
-      <c r="AD337" s="12"/>
-      <c r="AE337" s="12"/>
-      <c r="AF337" s="12"/>
-      <c r="AG337" s="12"/>
-      <c r="AH337" s="13"/>
+      <c r="AH337" s="6"/>
     </row>
     <row r="338" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A338">
@@ -34809,13 +33961,7 @@
       <c r="AA339" t="s">
         <v>36</v>
       </c>
-      <c r="AB339" s="12"/>
-      <c r="AC339" s="12"/>
-      <c r="AD339" s="12"/>
-      <c r="AE339" s="12"/>
-      <c r="AF339" s="12"/>
-      <c r="AG339" s="12"/>
-      <c r="AH339" s="13"/>
+      <c r="AH339" s="6"/>
     </row>
     <row r="340" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A340">
@@ -34900,13 +34046,7 @@
       <c r="AA340" t="s">
         <v>36</v>
       </c>
-      <c r="AB340" s="12"/>
-      <c r="AC340" s="12"/>
-      <c r="AD340" s="12"/>
-      <c r="AE340" s="12"/>
-      <c r="AF340" s="12"/>
-      <c r="AG340" s="12"/>
-      <c r="AH340" s="13"/>
+      <c r="AH340" s="6"/>
     </row>
     <row r="341" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A341">
@@ -35181,13 +34321,7 @@
       <c r="AA343" t="s">
         <v>36</v>
       </c>
-      <c r="AB343" s="12"/>
-      <c r="AC343" s="12"/>
-      <c r="AD343" s="12"/>
-      <c r="AE343" s="12"/>
-      <c r="AF343" s="12"/>
-      <c r="AG343" s="12"/>
-      <c r="AH343" s="13"/>
+      <c r="AH343" s="6"/>
     </row>
     <row r="344" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A344">
@@ -35272,13 +34406,7 @@
       <c r="AA344" t="s">
         <v>36</v>
       </c>
-      <c r="AB344" s="12"/>
-      <c r="AC344" s="12"/>
-      <c r="AD344" s="12"/>
-      <c r="AE344" s="12"/>
-      <c r="AF344" s="12"/>
-      <c r="AG344" s="12"/>
-      <c r="AH344" s="13"/>
+      <c r="AH344" s="6"/>
     </row>
     <row r="345" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A345">
@@ -35363,13 +34491,7 @@
       <c r="AA345" t="s">
         <v>36</v>
       </c>
-      <c r="AB345" s="12"/>
-      <c r="AC345" s="12"/>
-      <c r="AD345" s="12"/>
-      <c r="AE345" s="12"/>
-      <c r="AF345" s="12"/>
-      <c r="AG345" s="12"/>
-      <c r="AH345" s="13"/>
+      <c r="AH345" s="6"/>
     </row>
     <row r="346" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A346">
@@ -35549,17 +34671,13 @@
       <c r="AA347" t="s">
         <v>36</v>
       </c>
-      <c r="AB347" s="12"/>
-      <c r="AC347" s="12"/>
-      <c r="AD347" s="12"/>
-      <c r="AE347" s="12">
+      <c r="AE347">
         <v>1</v>
       </c>
-      <c r="AF347" s="12">
+      <c r="AF347">
         <v>1</v>
       </c>
-      <c r="AG347" s="12"/>
-      <c r="AH347" s="13"/>
+      <c r="AH347" s="6"/>
     </row>
     <row r="348" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A348">
@@ -35644,13 +34762,7 @@
       <c r="AA348" t="s">
         <v>36</v>
       </c>
-      <c r="AB348" s="12"/>
-      <c r="AC348" s="12"/>
-      <c r="AD348" s="12"/>
-      <c r="AE348" s="12"/>
-      <c r="AF348" s="12"/>
-      <c r="AG348" s="12"/>
-      <c r="AH348" s="13"/>
+      <c r="AH348" s="6"/>
     </row>
     <row r="349" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A349">
@@ -35735,15 +34847,10 @@
       <c r="AA349" t="s">
         <v>36</v>
       </c>
-      <c r="AB349" s="12"/>
-      <c r="AC349" s="12"/>
-      <c r="AD349" s="12">
+      <c r="AD349">
         <v>895</v>
       </c>
-      <c r="AE349" s="12"/>
-      <c r="AF349" s="12"/>
-      <c r="AG349" s="12"/>
-      <c r="AH349" s="13"/>
+      <c r="AH349" s="6"/>
     </row>
     <row r="350" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A350">
@@ -35923,13 +35030,7 @@
       <c r="AA351" t="s">
         <v>36</v>
       </c>
-      <c r="AB351" s="12"/>
-      <c r="AC351" s="12"/>
-      <c r="AD351" s="12"/>
-      <c r="AE351" s="12"/>
-      <c r="AF351" s="12"/>
-      <c r="AG351" s="12"/>
-      <c r="AH351" s="13"/>
+      <c r="AH351" s="6"/>
     </row>
     <row r="352" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A352">
@@ -36014,13 +35115,7 @@
       <c r="AA352" t="s">
         <v>36</v>
       </c>
-      <c r="AB352" s="12"/>
-      <c r="AC352" s="12"/>
-      <c r="AD352" s="12"/>
-      <c r="AE352" s="12"/>
-      <c r="AF352" s="12"/>
-      <c r="AG352" s="12"/>
-      <c r="AH352" s="13"/>
+      <c r="AH352" s="6"/>
     </row>
     <row r="353" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A353">
@@ -36105,15 +35200,10 @@
       <c r="AA353" t="s">
         <v>36</v>
       </c>
-      <c r="AB353" s="12"/>
-      <c r="AC353" s="12"/>
-      <c r="AD353" s="12">
+      <c r="AD353">
         <v>1330</v>
       </c>
-      <c r="AE353" s="12"/>
-      <c r="AF353" s="12"/>
-      <c r="AG353" s="12"/>
-      <c r="AH353" s="13"/>
+      <c r="AH353" s="6"/>
     </row>
     <row r="354" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A354">
@@ -36198,13 +35288,7 @@
       <c r="AA354" t="s">
         <v>36</v>
       </c>
-      <c r="AB354" s="12"/>
-      <c r="AC354" s="12"/>
-      <c r="AD354" s="12"/>
-      <c r="AE354" s="12"/>
-      <c r="AF354" s="12"/>
-      <c r="AG354" s="12"/>
-      <c r="AH354" s="13"/>
+      <c r="AH354" s="6"/>
     </row>
     <row r="355" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A355">
@@ -36289,13 +35373,7 @@
       <c r="AA355" t="s">
         <v>36</v>
       </c>
-      <c r="AB355" s="12"/>
-      <c r="AC355" s="12"/>
-      <c r="AD355" s="12"/>
-      <c r="AE355" s="12"/>
-      <c r="AF355" s="12"/>
-      <c r="AG355" s="12"/>
-      <c r="AH355" s="13"/>
+      <c r="AH355" s="6"/>
     </row>
     <row r="356" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A356">
@@ -36473,13 +35551,7 @@
       <c r="AA357" t="s">
         <v>36</v>
       </c>
-      <c r="AB357" s="12"/>
-      <c r="AC357" s="12"/>
-      <c r="AD357" s="12"/>
-      <c r="AE357" s="12"/>
-      <c r="AF357" s="12"/>
-      <c r="AG357" s="12"/>
-      <c r="AH357" s="13"/>
+      <c r="AH357" s="6"/>
     </row>
     <row r="358" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A358">
@@ -36564,13 +35636,7 @@
       <c r="AA358" t="s">
         <v>36</v>
       </c>
-      <c r="AB358" s="12"/>
-      <c r="AC358" s="12"/>
-      <c r="AD358" s="12"/>
-      <c r="AE358" s="12"/>
-      <c r="AF358" s="12"/>
-      <c r="AG358" s="12"/>
-      <c r="AH358" s="13"/>
+      <c r="AH358" s="6"/>
     </row>
     <row r="359" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A359">
@@ -36655,15 +35721,10 @@
       <c r="AA359" t="s">
         <v>36</v>
       </c>
-      <c r="AB359" s="12"/>
-      <c r="AC359" s="12"/>
-      <c r="AD359" s="12">
+      <c r="AD359">
         <v>1025</v>
       </c>
-      <c r="AE359" s="12"/>
-      <c r="AF359" s="12"/>
-      <c r="AG359" s="12"/>
-      <c r="AH359" s="13"/>
+      <c r="AH359" s="6"/>
     </row>
     <row r="360" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A360">
@@ -36748,13 +35809,7 @@
       <c r="AA360" t="s">
         <v>36</v>
       </c>
-      <c r="AB360" s="12"/>
-      <c r="AC360" s="12"/>
-      <c r="AD360" s="12"/>
-      <c r="AE360" s="12"/>
-      <c r="AF360" s="12"/>
-      <c r="AG360" s="12"/>
-      <c r="AH360" s="13"/>
+      <c r="AH360" s="6"/>
     </row>
     <row r="361" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A361">
@@ -36839,15 +35894,10 @@
       <c r="AA361" t="s">
         <v>36</v>
       </c>
-      <c r="AB361" s="12"/>
-      <c r="AC361" s="12"/>
-      <c r="AD361" s="12">
+      <c r="AD361">
         <v>730</v>
       </c>
-      <c r="AE361" s="12"/>
-      <c r="AF361" s="12"/>
-      <c r="AG361" s="12"/>
-      <c r="AH361" s="13"/>
+      <c r="AH361" s="6"/>
     </row>
     <row r="362" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A362">
@@ -36932,13 +35982,7 @@
       <c r="AA362" t="s">
         <v>36</v>
       </c>
-      <c r="AB362" s="12"/>
-      <c r="AC362" s="12"/>
-      <c r="AD362" s="12"/>
-      <c r="AE362" s="12"/>
-      <c r="AF362" s="12"/>
-      <c r="AG362" s="12"/>
-      <c r="AH362" s="13"/>
+      <c r="AH362" s="6"/>
     </row>
     <row r="363" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A363">
@@ -37023,13 +36067,7 @@
       <c r="AA363" t="s">
         <v>36</v>
       </c>
-      <c r="AB363" s="12"/>
-      <c r="AC363" s="12"/>
-      <c r="AD363" s="12"/>
-      <c r="AE363" s="12"/>
-      <c r="AF363" s="12"/>
-      <c r="AG363" s="12"/>
-      <c r="AH363" s="13"/>
+      <c r="AH363" s="6"/>
     </row>
     <row r="364" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A364">
@@ -37114,19 +36152,16 @@
       <c r="AA364" t="s">
         <v>36</v>
       </c>
-      <c r="AB364" s="12"/>
-      <c r="AC364" s="12"/>
-      <c r="AD364" s="12">
+      <c r="AD364">
         <v>1650</v>
       </c>
-      <c r="AE364" s="12">
+      <c r="AE364">
         <v>2</v>
       </c>
-      <c r="AF364" s="12">
+      <c r="AF364">
         <v>2</v>
       </c>
-      <c r="AG364" s="12"/>
-      <c r="AH364" s="13" t="s">
+      <c r="AH364" s="6" t="s">
         <v>1177</v>
       </c>
     </row>
@@ -37213,13 +36248,7 @@
       <c r="AA365" t="s">
         <v>36</v>
       </c>
-      <c r="AB365" s="12"/>
-      <c r="AC365" s="12"/>
-      <c r="AD365" s="12"/>
-      <c r="AE365" s="12"/>
-      <c r="AF365" s="12"/>
-      <c r="AG365" s="12"/>
-      <c r="AH365" s="13"/>
+      <c r="AH365" s="6"/>
     </row>
     <row r="366" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A366">
@@ -37304,13 +36333,7 @@
       <c r="AA366" t="s">
         <v>36</v>
       </c>
-      <c r="AB366" s="12"/>
-      <c r="AC366" s="12"/>
-      <c r="AD366" s="12"/>
-      <c r="AE366" s="12"/>
-      <c r="AF366" s="12"/>
-      <c r="AG366" s="12"/>
-      <c r="AH366" s="13"/>
+      <c r="AH366" s="6"/>
     </row>
     <row r="367" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A367">
@@ -37395,13 +36418,7 @@
       <c r="AA367" t="s">
         <v>36</v>
       </c>
-      <c r="AB367" s="12"/>
-      <c r="AC367" s="12"/>
-      <c r="AD367" s="12"/>
-      <c r="AE367" s="12"/>
-      <c r="AF367" s="12"/>
-      <c r="AG367" s="12"/>
-      <c r="AH367" s="13"/>
+      <c r="AH367" s="6"/>
     </row>
     <row r="368" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A368">
@@ -37486,13 +36503,7 @@
       <c r="AA368" t="s">
         <v>36</v>
       </c>
-      <c r="AB368" s="12"/>
-      <c r="AC368" s="12"/>
-      <c r="AD368" s="12"/>
-      <c r="AE368" s="12"/>
-      <c r="AF368" s="12"/>
-      <c r="AG368" s="12"/>
-      <c r="AH368" s="13"/>
+      <c r="AH368" s="6"/>
     </row>
     <row r="369" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A369">
@@ -37577,13 +36588,7 @@
       <c r="AA369" t="s">
         <v>36</v>
       </c>
-      <c r="AB369" s="12"/>
-      <c r="AC369" s="12"/>
-      <c r="AD369" s="12"/>
-      <c r="AE369" s="12"/>
-      <c r="AF369" s="12"/>
-      <c r="AG369" s="12"/>
-      <c r="AH369" s="13"/>
+      <c r="AH369" s="6"/>
     </row>
     <row r="370" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A370">
@@ -37668,15 +36673,10 @@
       <c r="AA370" t="s">
         <v>36</v>
       </c>
-      <c r="AB370" s="12"/>
-      <c r="AC370" s="12"/>
-      <c r="AD370" s="12">
+      <c r="AD370">
         <v>265</v>
       </c>
-      <c r="AE370" s="12"/>
-      <c r="AF370" s="12"/>
-      <c r="AG370" s="12"/>
-      <c r="AH370" s="13"/>
+      <c r="AH370" s="6"/>
     </row>
     <row r="371" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A371">
@@ -37856,13 +36856,7 @@
       <c r="AA372" t="s">
         <v>36</v>
       </c>
-      <c r="AB372" s="12"/>
-      <c r="AC372" s="12"/>
-      <c r="AD372" s="12"/>
-      <c r="AE372" s="12"/>
-      <c r="AF372" s="12"/>
-      <c r="AG372" s="12"/>
-      <c r="AH372" s="13"/>
+      <c r="AH372" s="6"/>
     </row>
     <row r="373" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A373">
@@ -37947,15 +36941,10 @@
       <c r="AA373" t="s">
         <v>36</v>
       </c>
-      <c r="AB373" s="12"/>
-      <c r="AC373" s="12"/>
-      <c r="AD373" s="12">
+      <c r="AD373">
         <v>195</v>
       </c>
-      <c r="AE373" s="12"/>
-      <c r="AF373" s="12"/>
-      <c r="AG373" s="12"/>
-      <c r="AH373" s="13"/>
+      <c r="AH373" s="6"/>
     </row>
     <row r="374" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A374">
@@ -38040,13 +37029,7 @@
       <c r="AA374" t="s">
         <v>36</v>
       </c>
-      <c r="AB374" s="12"/>
-      <c r="AC374" s="12"/>
-      <c r="AD374" s="12"/>
-      <c r="AE374" s="12"/>
-      <c r="AF374" s="12"/>
-      <c r="AG374" s="12"/>
-      <c r="AH374" s="13"/>
+      <c r="AH374" s="6"/>
     </row>
     <row r="375" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A375">
@@ -38131,13 +37114,7 @@
       <c r="AA375" t="s">
         <v>36</v>
       </c>
-      <c r="AB375" s="12"/>
-      <c r="AC375" s="12"/>
-      <c r="AD375" s="12"/>
-      <c r="AE375" s="12"/>
-      <c r="AF375" s="12"/>
-      <c r="AG375" s="12"/>
-      <c r="AH375" s="13"/>
+      <c r="AH375" s="6"/>
     </row>
     <row r="376" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A376">
@@ -38222,19 +37199,16 @@
       <c r="AA376" t="s">
         <v>36</v>
       </c>
-      <c r="AB376" s="12"/>
-      <c r="AC376" s="12"/>
-      <c r="AD376" s="12">
+      <c r="AD376">
         <v>1140</v>
       </c>
-      <c r="AE376" s="12">
+      <c r="AE376">
         <v>1</v>
       </c>
-      <c r="AF376" s="12">
+      <c r="AF376">
         <v>1</v>
       </c>
-      <c r="AG376" s="12"/>
-      <c r="AH376" s="13"/>
+      <c r="AH376" s="6"/>
     </row>
     <row r="377" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A377">
@@ -38319,13 +37293,7 @@
       <c r="AA377" t="s">
         <v>36</v>
       </c>
-      <c r="AB377" s="12"/>
-      <c r="AC377" s="12"/>
-      <c r="AD377" s="12"/>
-      <c r="AE377" s="12"/>
-      <c r="AF377" s="12"/>
-      <c r="AG377" s="12"/>
-      <c r="AH377" s="13"/>
+      <c r="AH377" s="6"/>
     </row>
     <row r="378" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A378">
@@ -38410,15 +37378,10 @@
       <c r="AA378" t="s">
         <v>36</v>
       </c>
-      <c r="AB378" s="12"/>
-      <c r="AC378" s="12"/>
-      <c r="AD378" s="12">
+      <c r="AD378">
         <v>2299</v>
       </c>
-      <c r="AE378" s="12"/>
-      <c r="AF378" s="12"/>
-      <c r="AG378" s="12"/>
-      <c r="AH378" s="13"/>
+      <c r="AH378" s="6"/>
     </row>
     <row r="379" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A379">
@@ -38503,13 +37466,7 @@
       <c r="AA379" t="s">
         <v>36</v>
       </c>
-      <c r="AB379" s="12"/>
-      <c r="AC379" s="12"/>
-      <c r="AD379" s="12"/>
-      <c r="AE379" s="12"/>
-      <c r="AF379" s="12"/>
-      <c r="AG379" s="12"/>
-      <c r="AH379" s="13"/>
+      <c r="AH379" s="6"/>
     </row>
     <row r="380" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A380">
@@ -38594,13 +37551,7 @@
       <c r="AA380" t="s">
         <v>36</v>
       </c>
-      <c r="AB380" s="12"/>
-      <c r="AC380" s="12"/>
-      <c r="AD380" s="12"/>
-      <c r="AE380" s="12"/>
-      <c r="AF380" s="12"/>
-      <c r="AG380" s="12"/>
-      <c r="AH380" s="13"/>
+      <c r="AH380" s="6"/>
     </row>
     <row r="381" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A381">
@@ -38685,13 +37636,7 @@
       <c r="AA381" t="s">
         <v>36</v>
       </c>
-      <c r="AB381" s="12"/>
-      <c r="AC381" s="12"/>
-      <c r="AD381" s="12"/>
-      <c r="AE381" s="12"/>
-      <c r="AF381" s="12"/>
-      <c r="AG381" s="12"/>
-      <c r="AH381" s="13"/>
+      <c r="AH381" s="6"/>
     </row>
     <row r="382" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A382">
@@ -38776,13 +37721,7 @@
       <c r="AA382" t="s">
         <v>36</v>
       </c>
-      <c r="AB382" s="12"/>
-      <c r="AC382" s="12"/>
-      <c r="AD382" s="12"/>
-      <c r="AE382" s="12"/>
-      <c r="AF382" s="12"/>
-      <c r="AG382" s="12"/>
-      <c r="AH382" s="13"/>
+      <c r="AH382" s="6"/>
     </row>
     <row r="383" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A383">
@@ -38867,17 +37806,13 @@
       <c r="AA383" t="s">
         <v>36</v>
       </c>
-      <c r="AB383" s="12"/>
-      <c r="AC383" s="12"/>
-      <c r="AD383" s="12"/>
-      <c r="AE383" s="12">
+      <c r="AE383">
         <v>1</v>
       </c>
-      <c r="AF383" s="12">
+      <c r="AF383">
         <v>1</v>
       </c>
-      <c r="AG383" s="12"/>
-      <c r="AH383" s="13"/>
+      <c r="AH383" s="6"/>
     </row>
     <row r="384" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A384">
@@ -38962,13 +37897,7 @@
       <c r="AA384" t="s">
         <v>36</v>
       </c>
-      <c r="AB384" s="12"/>
-      <c r="AC384" s="12"/>
-      <c r="AD384" s="12"/>
-      <c r="AE384" s="12"/>
-      <c r="AF384" s="12"/>
-      <c r="AG384" s="12"/>
-      <c r="AH384" s="13"/>
+      <c r="AH384" s="6"/>
     </row>
     <row r="385" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A385">
@@ -39053,13 +37982,7 @@
       <c r="AA385" t="s">
         <v>36</v>
       </c>
-      <c r="AB385" s="12"/>
-      <c r="AC385" s="12"/>
-      <c r="AD385" s="12"/>
-      <c r="AE385" s="12"/>
-      <c r="AF385" s="12"/>
-      <c r="AG385" s="12"/>
-      <c r="AH385" s="13"/>
+      <c r="AH385" s="6"/>
     </row>
     <row r="386" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A386">
@@ -39144,13 +38067,7 @@
       <c r="AA386" t="s">
         <v>36</v>
       </c>
-      <c r="AB386" s="12"/>
-      <c r="AC386" s="12"/>
-      <c r="AD386" s="12"/>
-      <c r="AE386" s="12"/>
-      <c r="AF386" s="12"/>
-      <c r="AG386" s="12"/>
-      <c r="AH386" s="13"/>
+      <c r="AH386" s="6"/>
     </row>
     <row r="387" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A387">
@@ -39330,13 +38247,7 @@
       <c r="AA388" t="s">
         <v>36</v>
       </c>
-      <c r="AB388" s="12"/>
-      <c r="AC388" s="12"/>
-      <c r="AD388" s="12"/>
-      <c r="AE388" s="12"/>
-      <c r="AF388" s="12"/>
-      <c r="AG388" s="12"/>
-      <c r="AH388" s="13"/>
+      <c r="AH388" s="6"/>
     </row>
     <row r="389" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A389">
@@ -39421,13 +38332,7 @@
       <c r="AA389" t="s">
         <v>36</v>
       </c>
-      <c r="AB389" s="12"/>
-      <c r="AC389" s="12"/>
-      <c r="AD389" s="12"/>
-      <c r="AE389" s="12"/>
-      <c r="AF389" s="12"/>
-      <c r="AG389" s="12"/>
-      <c r="AH389" s="13"/>
+      <c r="AH389" s="6"/>
     </row>
     <row r="390" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A390">
@@ -39512,13 +38417,7 @@
       <c r="AA390" t="s">
         <v>36</v>
       </c>
-      <c r="AB390" s="12"/>
-      <c r="AC390" s="12"/>
-      <c r="AD390" s="12"/>
-      <c r="AE390" s="12"/>
-      <c r="AF390" s="12"/>
-      <c r="AG390" s="12"/>
-      <c r="AH390" s="13"/>
+      <c r="AH390" s="6"/>
     </row>
     <row r="391" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A391">
@@ -39603,13 +38502,7 @@
       <c r="AA391" t="s">
         <v>36</v>
       </c>
-      <c r="AB391" s="12"/>
-      <c r="AC391" s="12"/>
-      <c r="AD391" s="12"/>
-      <c r="AE391" s="12"/>
-      <c r="AF391" s="12"/>
-      <c r="AG391" s="12"/>
-      <c r="AH391" s="13"/>
+      <c r="AH391" s="6"/>
     </row>
     <row r="392" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A392">
@@ -39694,13 +38587,7 @@
       <c r="AA392" t="s">
         <v>36</v>
       </c>
-      <c r="AB392" s="12"/>
-      <c r="AC392" s="12"/>
-      <c r="AD392" s="12"/>
-      <c r="AE392" s="12"/>
-      <c r="AF392" s="12"/>
-      <c r="AG392" s="12"/>
-      <c r="AH392" s="13"/>
+      <c r="AH392" s="6"/>
     </row>
     <row r="393" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A393">
@@ -39785,13 +38672,7 @@
       <c r="AA393" t="s">
         <v>36</v>
       </c>
-      <c r="AB393" s="12"/>
-      <c r="AC393" s="12"/>
-      <c r="AD393" s="12"/>
-      <c r="AE393" s="12"/>
-      <c r="AF393" s="12"/>
-      <c r="AG393" s="12"/>
-      <c r="AH393" s="13"/>
+      <c r="AH393" s="6"/>
     </row>
     <row r="394" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A394">
@@ -39876,15 +38757,10 @@
       <c r="AA394" t="s">
         <v>36</v>
       </c>
-      <c r="AB394" s="12"/>
-      <c r="AC394" s="12"/>
-      <c r="AD394" s="12">
+      <c r="AD394">
         <v>1358</v>
       </c>
-      <c r="AE394" s="12"/>
-      <c r="AF394" s="12"/>
-      <c r="AG394" s="12"/>
-      <c r="AH394" s="13"/>
+      <c r="AH394" s="6"/>
     </row>
     <row r="395" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A395">
@@ -39969,13 +38845,7 @@
       <c r="AA395" t="s">
         <v>36</v>
       </c>
-      <c r="AB395" s="12"/>
-      <c r="AC395" s="12"/>
-      <c r="AD395" s="12"/>
-      <c r="AE395" s="12"/>
-      <c r="AF395" s="12"/>
-      <c r="AG395" s="12"/>
-      <c r="AH395" s="13"/>
+      <c r="AH395" s="6"/>
     </row>
     <row r="396" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A396">
@@ -40155,13 +39025,7 @@
       <c r="AA397" t="s">
         <v>36</v>
       </c>
-      <c r="AB397" s="12"/>
-      <c r="AC397" s="12"/>
-      <c r="AD397" s="12"/>
-      <c r="AE397" s="12"/>
-      <c r="AF397" s="12"/>
-      <c r="AG397" s="12"/>
-      <c r="AH397" s="13"/>
+      <c r="AH397" s="6"/>
     </row>
     <row r="398" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A398">
@@ -40246,13 +39110,7 @@
       <c r="AA398" t="s">
         <v>36</v>
       </c>
-      <c r="AB398" s="12"/>
-      <c r="AC398" s="12"/>
-      <c r="AD398" s="12"/>
-      <c r="AE398" s="12"/>
-      <c r="AF398" s="12"/>
-      <c r="AG398" s="12"/>
-      <c r="AH398" s="13"/>
+      <c r="AH398" s="6"/>
     </row>
     <row r="399" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A399">
@@ -40337,13 +39195,7 @@
       <c r="AA399" t="s">
         <v>36</v>
       </c>
-      <c r="AB399" s="12"/>
-      <c r="AC399" s="12"/>
-      <c r="AD399" s="12"/>
-      <c r="AE399" s="12"/>
-      <c r="AF399" s="12"/>
-      <c r="AG399" s="12"/>
-      <c r="AH399" s="13"/>
+      <c r="AH399" s="6"/>
     </row>
     <row r="400" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A400">
@@ -40428,13 +39280,7 @@
       <c r="AA400" t="s">
         <v>36</v>
       </c>
-      <c r="AB400" s="12"/>
-      <c r="AC400" s="12"/>
-      <c r="AD400" s="12"/>
-      <c r="AE400" s="12"/>
-      <c r="AF400" s="12"/>
-      <c r="AG400" s="12"/>
-      <c r="AH400" s="13"/>
+      <c r="AH400" s="6"/>
     </row>
     <row r="401" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A401">
@@ -40519,13 +39365,7 @@
       <c r="AA401" t="s">
         <v>36</v>
       </c>
-      <c r="AB401" s="12"/>
-      <c r="AC401" s="12"/>
-      <c r="AD401" s="12"/>
-      <c r="AE401" s="12"/>
-      <c r="AF401" s="12"/>
-      <c r="AG401" s="12"/>
-      <c r="AH401" s="13"/>
+      <c r="AH401" s="6"/>
     </row>
     <row r="402" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A402">
@@ -40705,13 +39545,7 @@
       <c r="AA403" t="s">
         <v>36</v>
       </c>
-      <c r="AB403" s="12"/>
-      <c r="AC403" s="12"/>
-      <c r="AD403" s="12"/>
-      <c r="AE403" s="12"/>
-      <c r="AF403" s="12"/>
-      <c r="AG403" s="12"/>
-      <c r="AH403" s="13"/>
+      <c r="AH403" s="6"/>
     </row>
     <row r="404" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A404">
@@ -40796,13 +39630,7 @@
       <c r="AA404" t="s">
         <v>36</v>
       </c>
-      <c r="AB404" s="12"/>
-      <c r="AC404" s="12"/>
-      <c r="AD404" s="12"/>
-      <c r="AE404" s="12"/>
-      <c r="AF404" s="12"/>
-      <c r="AG404" s="12"/>
-      <c r="AH404" s="13"/>
+      <c r="AH404" s="6"/>
     </row>
     <row r="405" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A405">
@@ -40982,13 +39810,7 @@
       <c r="AA406" t="s">
         <v>36</v>
       </c>
-      <c r="AB406" s="12"/>
-      <c r="AC406" s="12"/>
-      <c r="AD406" s="12"/>
-      <c r="AE406" s="12"/>
-      <c r="AF406" s="12"/>
-      <c r="AG406" s="12"/>
-      <c r="AH406" s="13"/>
+      <c r="AH406" s="6"/>
     </row>
     <row r="407" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A407">
@@ -41073,13 +39895,7 @@
       <c r="AA407" t="s">
         <v>36</v>
       </c>
-      <c r="AB407" s="12"/>
-      <c r="AC407" s="12"/>
-      <c r="AD407" s="12"/>
-      <c r="AE407" s="12"/>
-      <c r="AF407" s="12"/>
-      <c r="AG407" s="12"/>
-      <c r="AH407" s="13"/>
+      <c r="AH407" s="6"/>
     </row>
     <row r="408" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A408">
@@ -41164,13 +39980,7 @@
       <c r="AA408" t="s">
         <v>36</v>
       </c>
-      <c r="AB408" s="12"/>
-      <c r="AC408" s="12"/>
-      <c r="AD408" s="12"/>
-      <c r="AE408" s="12"/>
-      <c r="AF408" s="12"/>
-      <c r="AG408" s="12"/>
-      <c r="AH408" s="13"/>
+      <c r="AH408" s="6"/>
     </row>
     <row r="409" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A409">
@@ -41255,13 +40065,7 @@
       <c r="AA409" t="s">
         <v>36</v>
       </c>
-      <c r="AB409" s="12"/>
-      <c r="AC409" s="12"/>
-      <c r="AD409" s="12"/>
-      <c r="AE409" s="12"/>
-      <c r="AF409" s="12"/>
-      <c r="AG409" s="12"/>
-      <c r="AH409" s="13"/>
+      <c r="AH409" s="6"/>
     </row>
     <row r="410" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A410">
@@ -41346,13 +40150,7 @@
       <c r="AA410" t="s">
         <v>36</v>
       </c>
-      <c r="AB410" s="12"/>
-      <c r="AC410" s="12"/>
-      <c r="AD410" s="12"/>
-      <c r="AE410" s="12"/>
-      <c r="AF410" s="12"/>
-      <c r="AG410" s="12"/>
-      <c r="AH410" s="13"/>
+      <c r="AH410" s="6"/>
     </row>
     <row r="411" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A411">
@@ -41437,13 +40235,7 @@
       <c r="AA411" t="s">
         <v>36</v>
       </c>
-      <c r="AB411" s="12"/>
-      <c r="AC411" s="12"/>
-      <c r="AD411" s="12"/>
-      <c r="AE411" s="12"/>
-      <c r="AF411" s="12"/>
-      <c r="AG411" s="12"/>
-      <c r="AH411" s="13"/>
+      <c r="AH411" s="6"/>
     </row>
     <row r="412" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A412">
@@ -41528,13 +40320,13 @@
       <c r="AA412" t="s">
         <v>36</v>
       </c>
-      <c r="AB412" s="17"/>
-      <c r="AC412" s="17"/>
-      <c r="AD412" s="17"/>
-      <c r="AE412" s="17"/>
-      <c r="AF412" s="17"/>
-      <c r="AG412" s="17"/>
-      <c r="AH412" s="18"/>
+      <c r="AB412" s="13"/>
+      <c r="AC412" s="13"/>
+      <c r="AD412" s="13"/>
+      <c r="AE412" s="13"/>
+      <c r="AF412" s="13"/>
+      <c r="AG412" s="13"/>
+      <c r="AH412" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="Y2:Y412">

</xml_diff>